<commit_message>
first test of github actions with published directory
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="172">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -896,7 +896,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="493">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1001,6 +1001,1311 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1298,12 +2603,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="29.71" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="31.29" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="8.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="25.71" collapsed="false"/>
-    <col min="6" max="25" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.71" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.29" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.71" collapsed="true"/>
+    <col min="6" max="25" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
@@ -4095,13 +5400,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.29" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.71" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="22.86" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="21.71" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="112.43" collapsed="false"/>
-    <col min="7" max="26" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.71" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.86" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.71" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="112.43" collapsed="true"/>
+    <col min="7" max="26" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -4155,42 +5460,42 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="348" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="350" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="352" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="354" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="356" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="358" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="349" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="351" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="353" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="355" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="357" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="359" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5260,17 +6565,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.71" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.43" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.43" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="8.43" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="28.43" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.43" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="8" max="9" customWidth="true" width="21.43" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="35.14" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="16.71" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="21.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="9.71" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.43" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.43" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.43" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.43" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="21.43" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="35.14" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.71" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="21.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -5344,25 +6649,25 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="360" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="365" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="370" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="375" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="380" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="385" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="390" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -5370,25 +6675,25 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="361" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="366" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="371" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="376" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="381" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="386" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="391" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -5396,25 +6701,25 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="362" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="367" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="372" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="54" t="s">
+      <c r="F5" s="377" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="382" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="387" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="392" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -5422,25 +6727,25 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="363" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="368" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="373" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="378" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="383" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="388" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="393" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -5448,25 +6753,25 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="364" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="369" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="374" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="379" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="384" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="389" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="394" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -6885,18 +8190,18 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.14" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="11.71" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.43" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.43" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="13.86" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.86" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="29.71" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="16.43" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="19.14" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="21.43" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="19.0" collapsed="false"/>
-    <col min="12" max="31" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.14" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.71" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.43" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.86" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.71" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.43" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.14" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.43" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="12" max="31" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -6992,31 +8297,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="395" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="406" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="417" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="427" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="438" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="449" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="460" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="471" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="482" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="9"/>
@@ -7030,31 +8335,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="396" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="407" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="418" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="428" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="439" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="450" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="461" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="54" t="s">
+      <c r="J4" s="472" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="54" t="s">
+      <c r="K4" s="483" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="9"/>
@@ -7068,31 +8373,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="397" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="408" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="419" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="54" t="s">
+      <c r="F5" s="429" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="440" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="451" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="462" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="54" t="s">
+      <c r="J5" s="473" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="K5" s="484" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="9"/>
@@ -7106,31 +8411,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="398" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="409" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="420" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="430" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="441" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="452" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="463" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="474" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="54" t="s">
+      <c r="K6" s="485" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="9"/>
@@ -7144,29 +8449,29 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="399" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="410" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="431" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="442" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="453" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="464" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="475" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="54" t="s">
+      <c r="K7" s="486" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="9"/>
@@ -7180,31 +8485,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="400" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="411" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="421" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="432" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="443" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="454" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="465" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="54" t="s">
+      <c r="J8" s="476" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="54" t="s">
+      <c r="K8" s="487" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="9"/>
@@ -7218,31 +8523,31 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="401" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="412" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="422" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="433" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="54" t="s">
+      <c r="G9" s="444" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="54" t="s">
+      <c r="H9" s="455" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="466" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="477" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="54" t="s">
+      <c r="K9" s="488" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="9"/>
@@ -7256,31 +8561,31 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="402" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="413" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="423" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="434" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="445" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="54" t="s">
+      <c r="H10" s="456" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="467" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="54" t="s">
+      <c r="J10" s="478" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="54" t="s">
+      <c r="K10" s="489" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="9"/>
@@ -7294,31 +8599,31 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="403" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="414" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="424" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="54" t="s">
+      <c r="F11" s="435" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="54" t="s">
+      <c r="G11" s="446" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="54" t="s">
+      <c r="H11" s="457" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="54" t="s">
+      <c r="I11" s="468" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="54" t="s">
+      <c r="J11" s="479" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="54" t="s">
+      <c r="K11" s="490" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="9"/>
@@ -7332,31 +8637,31 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="404" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="415" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="54" t="s">
+      <c r="E12" s="425" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="54" t="s">
+      <c r="F12" s="436" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="54" t="s">
+      <c r="G12" s="447" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="54" t="s">
+      <c r="H12" s="458" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="54" t="s">
+      <c r="I12" s="469" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="480" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="54" t="s">
+      <c r="K12" s="491" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="9"/>
@@ -7370,31 +8675,31 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="405" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="416" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="426" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="437" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="54" t="s">
+      <c r="G13" s="448" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="54" t="s">
+      <c r="H13" s="459" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="54" t="s">
+      <c r="I13" s="470" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="54" t="s">
+      <c r="J13" s="481" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="54" t="s">
+      <c r="K13" s="492" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="9"/>
@@ -9378,19 +10683,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.29" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.86" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.43" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="7.14" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="19.43" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.71" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.43" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="19.29" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.14" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="21.86" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="28.14" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="16.71" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="21.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.29" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.86" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="7.14" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.43" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.71" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.43" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.29" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.14" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.86" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.14" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.71" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="21.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.75" customHeight="1">
@@ -11017,19 +12322,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="8.29" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.29" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.43" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="10.29" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="39.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="22.43" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="17.43" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.43" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="16.43" collapsed="false"/>
-    <col min="12" max="13" customWidth="true" width="10.86" collapsed="false"/>
-    <col min="14" max="31" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.29" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.43" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.29" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.43" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.43" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.43" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.43" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="10.86" collapsed="true"/>
+    <col min="14" max="31" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -13358,17 +14663,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.43" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="10.29" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="8.86" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="16.43" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="64.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="38.43" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="16.86" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="14.29" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="20.43" collapsed="false"/>
-    <col min="10" max="12" customWidth="true" width="12.29" collapsed="false"/>
-    <col min="13" max="14" customWidth="true" width="16.29" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="9.43" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.86" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.43" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="64.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="38.43" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.86" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.29" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.43" collapsed="true"/>
+    <col min="10" max="12" customWidth="true" width="12.29" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="16.29" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
@@ -18012,8 +19317,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="150.0" collapsed="false"/>
-    <col min="2" max="6" customWidth="true" width="10.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="150.0" collapsed="true"/>
+    <col min="2" max="6" customWidth="true" width="10.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">

</xml_diff>

<commit_message>
including pics in published/ trying environmental variable in gh action
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="172">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -896,7 +896,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="493">
+  <cellXfs count="638">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1001,6 +1001,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -5460,42 +5895,42 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="348" t="s">
+      <c r="A3" s="493" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="350" t="s">
+      <c r="B3" s="495" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="352" t="s">
+      <c r="C3" s="497" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="354" t="s">
+      <c r="D3" s="499" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="356" t="s">
+      <c r="E3" s="501" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="358" t="s">
+      <c r="F3" s="503" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="349" t="s">
+      <c r="A4" s="494" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="351" t="s">
+      <c r="B4" s="496" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="353" t="s">
+      <c r="C4" s="498" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="355" t="s">
+      <c r="D4" s="500" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="357" t="s">
+      <c r="E4" s="502" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="359" t="s">
+      <c r="F4" s="504" t="s">
         <v>34</v>
       </c>
     </row>
@@ -6649,25 +7084,25 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="360" t="s">
+      <c r="C3" s="505" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="365" t="s">
+      <c r="D3" s="510" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="370" t="s">
+      <c r="E3" s="515" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="375" t="s">
+      <c r="F3" s="520" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="380" t="s">
+      <c r="G3" s="525" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="385" t="s">
+      <c r="H3" s="530" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="390" t="s">
+      <c r="I3" s="535" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -6675,25 +7110,25 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="361" t="s">
+      <c r="C4" s="506" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="366" t="s">
+      <c r="D4" s="511" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="371" t="s">
+      <c r="E4" s="516" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="376" t="s">
+      <c r="F4" s="521" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="381" t="s">
+      <c r="G4" s="526" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="386" t="s">
+      <c r="H4" s="531" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="391" t="s">
+      <c r="I4" s="536" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -6701,25 +7136,25 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="362" t="s">
+      <c r="C5" s="507" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="367" t="s">
+      <c r="D5" s="512" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="372" t="s">
+      <c r="E5" s="517" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="377" t="s">
+      <c r="F5" s="522" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="382" t="s">
+      <c r="G5" s="527" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="387" t="s">
+      <c r="H5" s="532" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="392" t="s">
+      <c r="I5" s="537" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -6727,25 +7162,25 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="363" t="s">
+      <c r="C6" s="508" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="368" t="s">
+      <c r="D6" s="513" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="373" t="s">
+      <c r="E6" s="518" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="378" t="s">
+      <c r="F6" s="523" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="383" t="s">
+      <c r="G6" s="528" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="388" t="s">
+      <c r="H6" s="533" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="393" t="s">
+      <c r="I6" s="538" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -6753,25 +7188,25 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="364" t="s">
+      <c r="C7" s="509" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="369" t="s">
+      <c r="D7" s="514" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="374" t="s">
+      <c r="E7" s="519" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="379" t="s">
+      <c r="F7" s="524" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="384" t="s">
+      <c r="G7" s="529" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="389" t="s">
+      <c r="H7" s="534" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="394" t="s">
+      <c r="I7" s="539" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -8297,31 +8732,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="395" t="s">
+      <c r="C3" s="540" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="406" t="s">
+      <c r="D3" s="551" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="417" t="s">
+      <c r="E3" s="562" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="427" t="s">
+      <c r="F3" s="572" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="438" t="s">
+      <c r="G3" s="583" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="449" t="s">
+      <c r="H3" s="594" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="460" t="s">
+      <c r="I3" s="605" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="471" t="s">
+      <c r="J3" s="616" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="482" t="s">
+      <c r="K3" s="627" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="9"/>
@@ -8335,31 +8770,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="396" t="s">
+      <c r="C4" s="541" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="407" t="s">
+      <c r="D4" s="552" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="418" t="s">
+      <c r="E4" s="563" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="428" t="s">
+      <c r="F4" s="573" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="439" t="s">
+      <c r="G4" s="584" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="450" t="s">
+      <c r="H4" s="595" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="461" t="s">
+      <c r="I4" s="606" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="472" t="s">
+      <c r="J4" s="617" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="483" t="s">
+      <c r="K4" s="628" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="9"/>
@@ -8373,31 +8808,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="397" t="s">
+      <c r="C5" s="542" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="408" t="s">
+      <c r="D5" s="553" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="419" t="s">
+      <c r="E5" s="564" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="429" t="s">
+      <c r="F5" s="574" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="440" t="s">
+      <c r="G5" s="585" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="451" t="s">
+      <c r="H5" s="596" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="462" t="s">
+      <c r="I5" s="607" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="473" t="s">
+      <c r="J5" s="618" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="484" t="s">
+      <c r="K5" s="629" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="9"/>
@@ -8411,31 +8846,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="398" t="s">
+      <c r="C6" s="543" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="409" t="s">
+      <c r="D6" s="554" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="420" t="s">
+      <c r="E6" s="565" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="430" t="s">
+      <c r="F6" s="575" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="441" t="s">
+      <c r="G6" s="586" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="452" t="s">
+      <c r="H6" s="597" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="463" t="s">
+      <c r="I6" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="474" t="s">
+      <c r="J6" s="619" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="485" t="s">
+      <c r="K6" s="630" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="9"/>
@@ -8449,29 +8884,29 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="399" t="s">
+      <c r="C7" s="544" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="410" t="s">
+      <c r="D7" s="555" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="431" t="s">
+      <c r="F7" s="576" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="442" t="s">
+      <c r="G7" s="587" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="453" t="s">
+      <c r="H7" s="598" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="464" t="s">
+      <c r="I7" s="609" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="475" t="s">
+      <c r="J7" s="620" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="486" t="s">
+      <c r="K7" s="631" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="9"/>
@@ -8485,31 +8920,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="400" t="s">
+      <c r="C8" s="545" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="411" t="s">
+      <c r="D8" s="556" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="421" t="s">
+      <c r="E8" s="566" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="432" t="s">
+      <c r="F8" s="577" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="443" t="s">
+      <c r="G8" s="588" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="454" t="s">
+      <c r="H8" s="599" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="465" t="s">
+      <c r="I8" s="610" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="476" t="s">
+      <c r="J8" s="621" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="487" t="s">
+      <c r="K8" s="632" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="9"/>
@@ -8523,31 +8958,31 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="401" t="s">
+      <c r="C9" s="546" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="412" t="s">
+      <c r="D9" s="557" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="422" t="s">
+      <c r="E9" s="567" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="433" t="s">
+      <c r="F9" s="578" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="444" t="s">
+      <c r="G9" s="589" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="455" t="s">
+      <c r="H9" s="600" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="466" t="s">
+      <c r="I9" s="611" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="477" t="s">
+      <c r="J9" s="622" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="488" t="s">
+      <c r="K9" s="633" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="9"/>
@@ -8561,31 +8996,31 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="402" t="s">
+      <c r="C10" s="547" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="413" t="s">
+      <c r="D10" s="558" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="423" t="s">
+      <c r="E10" s="568" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="434" t="s">
+      <c r="F10" s="579" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="445" t="s">
+      <c r="G10" s="590" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="456" t="s">
+      <c r="H10" s="601" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="467" t="s">
+      <c r="I10" s="612" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="478" t="s">
+      <c r="J10" s="623" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="489" t="s">
+      <c r="K10" s="634" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="9"/>
@@ -8599,31 +9034,31 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="403" t="s">
+      <c r="C11" s="548" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="414" t="s">
+      <c r="D11" s="559" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="424" t="s">
+      <c r="E11" s="569" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="435" t="s">
+      <c r="F11" s="580" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="446" t="s">
+      <c r="G11" s="591" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="457" t="s">
+      <c r="H11" s="602" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="468" t="s">
+      <c r="I11" s="613" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="479" t="s">
+      <c r="J11" s="624" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="490" t="s">
+      <c r="K11" s="635" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="9"/>
@@ -8637,31 +9072,31 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="404" t="s">
+      <c r="C12" s="549" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="415" t="s">
+      <c r="D12" s="560" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="425" t="s">
+      <c r="E12" s="570" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="436" t="s">
+      <c r="F12" s="581" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="447" t="s">
+      <c r="G12" s="592" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="458" t="s">
+      <c r="H12" s="603" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="469" t="s">
+      <c r="I12" s="614" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="480" t="s">
+      <c r="J12" s="625" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="491" t="s">
+      <c r="K12" s="636" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="9"/>
@@ -8675,31 +9110,31 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="405" t="s">
+      <c r="C13" s="550" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="416" t="s">
+      <c r="D13" s="561" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="426" t="s">
+      <c r="E13" s="571" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="437" t="s">
+      <c r="F13" s="582" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="448" t="s">
+      <c r="G13" s="593" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="459" t="s">
+      <c r="H13" s="604" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="470" t="s">
+      <c r="I13" s="615" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="481" t="s">
+      <c r="J13" s="626" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="492" t="s">
+      <c r="K13" s="637" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="9"/>

</xml_diff>

<commit_message>
changed build to clean target directory...should remove banner.png and screenshot
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="172">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -896,7 +896,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="638">
+  <cellXfs count="783">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1001,6 +1001,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -5895,42 +6330,42 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="493" t="s">
+      <c r="A3" s="638" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="495" t="s">
+      <c r="B3" s="640" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="497" t="s">
+      <c r="C3" s="642" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="499" t="s">
+      <c r="D3" s="644" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="501" t="s">
+      <c r="E3" s="646" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="503" t="s">
+      <c r="F3" s="648" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="494" t="s">
+      <c r="A4" s="639" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="496" t="s">
+      <c r="B4" s="641" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="498" t="s">
+      <c r="C4" s="643" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="500" t="s">
+      <c r="D4" s="645" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="502" t="s">
+      <c r="E4" s="647" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="504" t="s">
+      <c r="F4" s="649" t="s">
         <v>34</v>
       </c>
     </row>
@@ -7084,25 +7519,25 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="505" t="s">
+      <c r="C3" s="650" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="510" t="s">
+      <c r="D3" s="655" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="515" t="s">
+      <c r="E3" s="660" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="520" t="s">
+      <c r="F3" s="665" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="525" t="s">
+      <c r="G3" s="670" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="530" t="s">
+      <c r="H3" s="675" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="535" t="s">
+      <c r="I3" s="680" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -7110,25 +7545,25 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="506" t="s">
+      <c r="C4" s="651" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="511" t="s">
+      <c r="D4" s="656" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="516" t="s">
+      <c r="E4" s="661" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="521" t="s">
+      <c r="F4" s="666" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="526" t="s">
+      <c r="G4" s="671" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="531" t="s">
+      <c r="H4" s="676" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="536" t="s">
+      <c r="I4" s="681" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -7136,25 +7571,25 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="507" t="s">
+      <c r="C5" s="652" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="512" t="s">
+      <c r="D5" s="657" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="517" t="s">
+      <c r="E5" s="662" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="522" t="s">
+      <c r="F5" s="667" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="527" t="s">
+      <c r="G5" s="672" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="532" t="s">
+      <c r="H5" s="677" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="537" t="s">
+      <c r="I5" s="682" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -7162,25 +7597,25 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="508" t="s">
+      <c r="C6" s="653" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="513" t="s">
+      <c r="D6" s="658" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="518" t="s">
+      <c r="E6" s="663" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="523" t="s">
+      <c r="F6" s="668" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="528" t="s">
+      <c r="G6" s="673" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="533" t="s">
+      <c r="H6" s="678" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="538" t="s">
+      <c r="I6" s="683" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -7188,25 +7623,25 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="509" t="s">
+      <c r="C7" s="654" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="514" t="s">
+      <c r="D7" s="659" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="519" t="s">
+      <c r="E7" s="664" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="524" t="s">
+      <c r="F7" s="669" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="529" t="s">
+      <c r="G7" s="674" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="534" t="s">
+      <c r="H7" s="679" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="539" t="s">
+      <c r="I7" s="684" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -8732,31 +9167,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="540" t="s">
+      <c r="C3" s="685" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="551" t="s">
+      <c r="D3" s="696" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="562" t="s">
+      <c r="E3" s="707" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="572" t="s">
+      <c r="F3" s="717" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="583" t="s">
+      <c r="G3" s="728" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="594" t="s">
+      <c r="H3" s="739" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="605" t="s">
+      <c r="I3" s="750" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="616" t="s">
+      <c r="J3" s="761" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="627" t="s">
+      <c r="K3" s="772" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="9"/>
@@ -8770,31 +9205,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="541" t="s">
+      <c r="C4" s="686" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="552" t="s">
+      <c r="D4" s="697" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="563" t="s">
+      <c r="E4" s="708" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="573" t="s">
+      <c r="F4" s="718" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="584" t="s">
+      <c r="G4" s="729" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="595" t="s">
+      <c r="H4" s="740" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="606" t="s">
+      <c r="I4" s="751" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="617" t="s">
+      <c r="J4" s="762" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="628" t="s">
+      <c r="K4" s="773" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="9"/>
@@ -8808,31 +9243,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="542" t="s">
+      <c r="C5" s="687" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="553" t="s">
+      <c r="D5" s="698" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="564" t="s">
+      <c r="E5" s="709" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="574" t="s">
+      <c r="F5" s="719" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="585" t="s">
+      <c r="G5" s="730" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="596" t="s">
+      <c r="H5" s="741" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="607" t="s">
+      <c r="I5" s="752" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="618" t="s">
+      <c r="J5" s="763" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="629" t="s">
+      <c r="K5" s="774" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="9"/>
@@ -8846,31 +9281,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="543" t="s">
+      <c r="C6" s="688" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="554" t="s">
+      <c r="D6" s="699" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="565" t="s">
+      <c r="E6" s="710" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="575" t="s">
+      <c r="F6" s="720" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="586" t="s">
+      <c r="G6" s="731" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="597" t="s">
+      <c r="H6" s="742" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="608" t="s">
+      <c r="I6" s="753" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="619" t="s">
+      <c r="J6" s="764" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="630" t="s">
+      <c r="K6" s="775" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="9"/>
@@ -8884,29 +9319,29 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="544" t="s">
+      <c r="C7" s="689" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="555" t="s">
+      <c r="D7" s="700" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="576" t="s">
+      <c r="F7" s="721" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="587" t="s">
+      <c r="G7" s="732" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="598" t="s">
+      <c r="H7" s="743" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="609" t="s">
+      <c r="I7" s="754" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="620" t="s">
+      <c r="J7" s="765" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="631" t="s">
+      <c r="K7" s="776" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="9"/>
@@ -8920,31 +9355,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="545" t="s">
+      <c r="C8" s="690" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="556" t="s">
+      <c r="D8" s="701" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="566" t="s">
+      <c r="E8" s="711" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="577" t="s">
+      <c r="F8" s="722" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="588" t="s">
+      <c r="G8" s="733" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="599" t="s">
+      <c r="H8" s="744" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="610" t="s">
+      <c r="I8" s="755" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="621" t="s">
+      <c r="J8" s="766" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="632" t="s">
+      <c r="K8" s="777" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="9"/>
@@ -8958,31 +9393,31 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="546" t="s">
+      <c r="C9" s="691" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="557" t="s">
+      <c r="D9" s="702" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="567" t="s">
+      <c r="E9" s="712" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="578" t="s">
+      <c r="F9" s="723" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="589" t="s">
+      <c r="G9" s="734" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="600" t="s">
+      <c r="H9" s="745" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="611" t="s">
+      <c r="I9" s="756" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="622" t="s">
+      <c r="J9" s="767" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="633" t="s">
+      <c r="K9" s="778" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="9"/>
@@ -8996,31 +9431,31 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="547" t="s">
+      <c r="C10" s="692" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="558" t="s">
+      <c r="D10" s="703" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="568" t="s">
+      <c r="E10" s="713" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="579" t="s">
+      <c r="F10" s="724" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="590" t="s">
+      <c r="G10" s="735" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="601" t="s">
+      <c r="H10" s="746" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="612" t="s">
+      <c r="I10" s="757" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="623" t="s">
+      <c r="J10" s="768" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="634" t="s">
+      <c r="K10" s="779" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="9"/>
@@ -9034,31 +9469,31 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="548" t="s">
+      <c r="C11" s="693" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="559" t="s">
+      <c r="D11" s="704" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="569" t="s">
+      <c r="E11" s="714" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="580" t="s">
+      <c r="F11" s="725" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="591" t="s">
+      <c r="G11" s="736" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="602" t="s">
+      <c r="H11" s="747" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="613" t="s">
+      <c r="I11" s="758" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="624" t="s">
+      <c r="J11" s="769" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="635" t="s">
+      <c r="K11" s="780" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="9"/>
@@ -9072,31 +9507,31 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="549" t="s">
+      <c r="C12" s="694" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="560" t="s">
+      <c r="D12" s="705" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="570" t="s">
+      <c r="E12" s="715" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="581" t="s">
+      <c r="F12" s="726" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="592" t="s">
+      <c r="G12" s="737" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="603" t="s">
+      <c r="H12" s="748" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="614" t="s">
+      <c r="I12" s="759" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="625" t="s">
+      <c r="J12" s="770" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="636" t="s">
+      <c r="K12" s="781" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="9"/>
@@ -9110,31 +9545,31 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="550" t="s">
+      <c r="C13" s="695" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="561" t="s">
+      <c r="D13" s="706" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="571" t="s">
+      <c r="E13" s="716" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="582" t="s">
+      <c r="F13" s="727" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="593" t="s">
+      <c r="G13" s="738" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="604" t="s">
+      <c r="H13" s="749" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="615" t="s">
+      <c r="I13" s="760" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="626" t="s">
+      <c r="J13" s="771" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="637" t="s">
+      <c r="K13" s="782" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="9"/>

</xml_diff>

<commit_message>
adjusted {} to null in lesson.json tweaked header of lesson.json to have galacticPubsVer
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="172">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -896,7 +896,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="783">
+  <cellXfs count="928">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1001,6 +1001,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -6330,42 +6765,42 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="638" t="s">
+      <c r="A3" s="783" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="640" t="s">
+      <c r="B3" s="785" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="642" t="s">
+      <c r="C3" s="787" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="644" t="s">
+      <c r="D3" s="789" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="646" t="s">
+      <c r="E3" s="791" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="648" t="s">
+      <c r="F3" s="793" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="639" t="s">
+      <c r="A4" s="784" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="641" t="s">
+      <c r="B4" s="786" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="643" t="s">
+      <c r="C4" s="788" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="645" t="s">
+      <c r="D4" s="790" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="647" t="s">
+      <c r="E4" s="792" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="649" t="s">
+      <c r="F4" s="794" t="s">
         <v>34</v>
       </c>
     </row>
@@ -7519,25 +7954,25 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="650" t="s">
+      <c r="C3" s="795" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="655" t="s">
+      <c r="D3" s="800" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="660" t="s">
+      <c r="E3" s="805" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="665" t="s">
+      <c r="F3" s="810" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="670" t="s">
+      <c r="G3" s="815" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="820" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="680" t="s">
+      <c r="I3" s="825" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -7545,25 +7980,25 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="651" t="s">
+      <c r="C4" s="796" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="656" t="s">
+      <c r="D4" s="801" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="661" t="s">
+      <c r="E4" s="806" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="666" t="s">
+      <c r="F4" s="811" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="671" t="s">
+      <c r="G4" s="816" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="676" t="s">
+      <c r="H4" s="821" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="681" t="s">
+      <c r="I4" s="826" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -7571,25 +8006,25 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="652" t="s">
+      <c r="C5" s="797" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="657" t="s">
+      <c r="D5" s="802" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="662" t="s">
+      <c r="E5" s="807" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="667" t="s">
+      <c r="F5" s="812" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="672" t="s">
+      <c r="G5" s="817" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="677" t="s">
+      <c r="H5" s="822" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="682" t="s">
+      <c r="I5" s="827" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -7597,25 +8032,25 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="653" t="s">
+      <c r="C6" s="798" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="658" t="s">
+      <c r="D6" s="803" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="663" t="s">
+      <c r="E6" s="808" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="668" t="s">
+      <c r="F6" s="813" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="673" t="s">
+      <c r="G6" s="818" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="678" t="s">
+      <c r="H6" s="823" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="683" t="s">
+      <c r="I6" s="828" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -7623,25 +8058,25 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="654" t="s">
+      <c r="C7" s="799" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="659" t="s">
+      <c r="D7" s="804" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="664" t="s">
+      <c r="E7" s="809" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="669" t="s">
+      <c r="F7" s="814" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="674" t="s">
+      <c r="G7" s="819" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="679" t="s">
+      <c r="H7" s="824" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="684" t="s">
+      <c r="I7" s="829" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -9167,31 +9602,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="685" t="s">
+      <c r="C3" s="830" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="696" t="s">
+      <c r="D3" s="841" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="707" t="s">
+      <c r="E3" s="852" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="717" t="s">
+      <c r="F3" s="862" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="728" t="s">
+      <c r="G3" s="873" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="739" t="s">
+      <c r="H3" s="884" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="750" t="s">
+      <c r="I3" s="895" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="761" t="s">
+      <c r="J3" s="906" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="772" t="s">
+      <c r="K3" s="917" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="9"/>
@@ -9205,31 +9640,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="686" t="s">
+      <c r="C4" s="831" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="697" t="s">
+      <c r="D4" s="842" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="708" t="s">
+      <c r="E4" s="853" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="718" t="s">
+      <c r="F4" s="863" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="729" t="s">
+      <c r="G4" s="874" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="740" t="s">
+      <c r="H4" s="885" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="751" t="s">
+      <c r="I4" s="896" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="762" t="s">
+      <c r="J4" s="907" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="773" t="s">
+      <c r="K4" s="918" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="9"/>
@@ -9243,31 +9678,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="687" t="s">
+      <c r="C5" s="832" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="698" t="s">
+      <c r="D5" s="843" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="709" t="s">
+      <c r="E5" s="854" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="719" t="s">
+      <c r="F5" s="864" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="730" t="s">
+      <c r="G5" s="875" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="741" t="s">
+      <c r="H5" s="886" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="752" t="s">
+      <c r="I5" s="897" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="763" t="s">
+      <c r="J5" s="908" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="774" t="s">
+      <c r="K5" s="919" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="9"/>
@@ -9281,31 +9716,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="688" t="s">
+      <c r="C6" s="833" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="699" t="s">
+      <c r="D6" s="844" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="710" t="s">
+      <c r="E6" s="855" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="720" t="s">
+      <c r="F6" s="865" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="731" t="s">
+      <c r="G6" s="876" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="742" t="s">
+      <c r="H6" s="887" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="753" t="s">
+      <c r="I6" s="898" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="764" t="s">
+      <c r="J6" s="909" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="775" t="s">
+      <c r="K6" s="920" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="9"/>
@@ -9319,29 +9754,29 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="689" t="s">
+      <c r="C7" s="834" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="700" t="s">
+      <c r="D7" s="845" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="721" t="s">
+      <c r="F7" s="866" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="732" t="s">
+      <c r="G7" s="877" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="743" t="s">
+      <c r="H7" s="888" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="754" t="s">
+      <c r="I7" s="899" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="765" t="s">
+      <c r="J7" s="910" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="776" t="s">
+      <c r="K7" s="921" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="9"/>
@@ -9355,31 +9790,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="690" t="s">
+      <c r="C8" s="835" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="701" t="s">
+      <c r="D8" s="846" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="711" t="s">
+      <c r="E8" s="856" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="722" t="s">
+      <c r="F8" s="867" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="733" t="s">
+      <c r="G8" s="878" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="744" t="s">
+      <c r="H8" s="889" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="755" t="s">
+      <c r="I8" s="900" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="766" t="s">
+      <c r="J8" s="911" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="777" t="s">
+      <c r="K8" s="922" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="9"/>
@@ -9393,31 +9828,31 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="691" t="s">
+      <c r="C9" s="836" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="702" t="s">
+      <c r="D9" s="847" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="712" t="s">
+      <c r="E9" s="857" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="723" t="s">
+      <c r="F9" s="868" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="734" t="s">
+      <c r="G9" s="879" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="745" t="s">
+      <c r="H9" s="890" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="756" t="s">
+      <c r="I9" s="901" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="767" t="s">
+      <c r="J9" s="912" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="778" t="s">
+      <c r="K9" s="923" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="9"/>
@@ -9431,31 +9866,31 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="692" t="s">
+      <c r="C10" s="837" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="703" t="s">
+      <c r="D10" s="848" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="713" t="s">
+      <c r="E10" s="858" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="724" t="s">
+      <c r="F10" s="869" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="735" t="s">
+      <c r="G10" s="880" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="746" t="s">
+      <c r="H10" s="891" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="757" t="s">
+      <c r="I10" s="902" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="768" t="s">
+      <c r="J10" s="913" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="779" t="s">
+      <c r="K10" s="924" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="9"/>
@@ -9469,31 +9904,31 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="693" t="s">
+      <c r="C11" s="838" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="704" t="s">
+      <c r="D11" s="849" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="714" t="s">
+      <c r="E11" s="859" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="725" t="s">
+      <c r="F11" s="870" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="736" t="s">
+      <c r="G11" s="881" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="747" t="s">
+      <c r="H11" s="892" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="758" t="s">
+      <c r="I11" s="903" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="769" t="s">
+      <c r="J11" s="914" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="780" t="s">
+      <c r="K11" s="925" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="9"/>
@@ -9507,31 +9942,31 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="694" t="s">
+      <c r="C12" s="839" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="705" t="s">
+      <c r="D12" s="850" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="715" t="s">
+      <c r="E12" s="860" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="726" t="s">
+      <c r="F12" s="871" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="737" t="s">
+      <c r="G12" s="882" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="748" t="s">
+      <c r="H12" s="893" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="759" t="s">
+      <c r="I12" s="904" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="770" t="s">
+      <c r="J12" s="915" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="781" t="s">
+      <c r="K12" s="926" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="9"/>
@@ -9545,31 +9980,31 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="695" t="s">
+      <c r="C13" s="840" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="706" t="s">
+      <c r="D13" s="851" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="716" t="s">
+      <c r="E13" s="861" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="727" t="s">
+      <c r="F13" s="872" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="738" t="s">
+      <c r="G13" s="883" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="749" t="s">
+      <c r="H13" s="894" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="760" t="s">
+      <c r="I13" s="905" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="771" t="s">
+      <c r="J13" s="916" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="782" t="s">
+      <c r="K13" s="927" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="9"/>

</xml_diff>

<commit_message>
updated using new infrastructure to expand relative paths to bundled assets to full catalog links
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="172">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -896,7 +896,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="928">
+  <cellXfs count="1073">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1001,6 +1001,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -6765,42 +7200,42 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="783" t="s">
+      <c r="A3" s="928" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="785" t="s">
+      <c r="B3" s="930" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="787" t="s">
+      <c r="C3" s="932" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="789" t="s">
+      <c r="D3" s="934" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="791" t="s">
+      <c r="E3" s="936" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="793" t="s">
+      <c r="F3" s="938" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="784" t="s">
+      <c r="A4" s="929" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="786" t="s">
+      <c r="B4" s="931" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="788" t="s">
+      <c r="C4" s="933" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="790" t="s">
+      <c r="D4" s="935" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="792" t="s">
+      <c r="E4" s="937" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="794" t="s">
+      <c r="F4" s="939" t="s">
         <v>34</v>
       </c>
     </row>
@@ -7954,25 +8389,25 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="795" t="s">
+      <c r="C3" s="940" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="800" t="s">
+      <c r="D3" s="945" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="805" t="s">
+      <c r="E3" s="950" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="810" t="s">
+      <c r="F3" s="955" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="815" t="s">
+      <c r="G3" s="960" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="820" t="s">
+      <c r="H3" s="965" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="825" t="s">
+      <c r="I3" s="970" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -7980,25 +8415,25 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="796" t="s">
+      <c r="C4" s="941" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="801" t="s">
+      <c r="D4" s="946" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="806" t="s">
+      <c r="E4" s="951" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="811" t="s">
+      <c r="F4" s="956" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="816" t="s">
+      <c r="G4" s="961" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="821" t="s">
+      <c r="H4" s="966" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="826" t="s">
+      <c r="I4" s="971" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -8006,25 +8441,25 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="797" t="s">
+      <c r="C5" s="942" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="802" t="s">
+      <c r="D5" s="947" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="807" t="s">
+      <c r="E5" s="952" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="812" t="s">
+      <c r="F5" s="957" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="817" t="s">
+      <c r="G5" s="962" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="822" t="s">
+      <c r="H5" s="967" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="827" t="s">
+      <c r="I5" s="972" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -8032,25 +8467,25 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="798" t="s">
+      <c r="C6" s="943" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="803" t="s">
+      <c r="D6" s="948" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="808" t="s">
+      <c r="E6" s="953" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="813" t="s">
+      <c r="F6" s="958" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="818" t="s">
+      <c r="G6" s="963" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="823" t="s">
+      <c r="H6" s="968" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="828" t="s">
+      <c r="I6" s="973" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -8058,25 +8493,25 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="799" t="s">
+      <c r="C7" s="944" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="804" t="s">
+      <c r="D7" s="949" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="809" t="s">
+      <c r="E7" s="954" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="814" t="s">
+      <c r="F7" s="959" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="819" t="s">
+      <c r="G7" s="964" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="824" t="s">
+      <c r="H7" s="969" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="829" t="s">
+      <c r="I7" s="974" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -9602,31 +10037,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="830" t="s">
+      <c r="C3" s="975" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="841" t="s">
+      <c r="D3" s="986" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="852" t="s">
+      <c r="E3" s="997" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="862" t="s">
+      <c r="F3" s="1007" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="873" t="s">
+      <c r="G3" s="1018" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="884" t="s">
+      <c r="H3" s="1029" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="895" t="s">
+      <c r="I3" s="1040" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="906" t="s">
+      <c r="J3" s="1051" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="917" t="s">
+      <c r="K3" s="1062" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="9"/>
@@ -9640,31 +10075,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="831" t="s">
+      <c r="C4" s="976" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="842" t="s">
+      <c r="D4" s="987" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="853" t="s">
+      <c r="E4" s="998" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="863" t="s">
+      <c r="F4" s="1008" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="874" t="s">
+      <c r="G4" s="1019" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="885" t="s">
+      <c r="H4" s="1030" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="896" t="s">
+      <c r="I4" s="1041" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="907" t="s">
+      <c r="J4" s="1052" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="918" t="s">
+      <c r="K4" s="1063" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="9"/>
@@ -9678,31 +10113,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="832" t="s">
+      <c r="C5" s="977" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="843" t="s">
+      <c r="D5" s="988" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="854" t="s">
+      <c r="E5" s="999" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="864" t="s">
+      <c r="F5" s="1009" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="875" t="s">
+      <c r="G5" s="1020" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="886" t="s">
+      <c r="H5" s="1031" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="897" t="s">
+      <c r="I5" s="1042" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="908" t="s">
+      <c r="J5" s="1053" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="919" t="s">
+      <c r="K5" s="1064" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="9"/>
@@ -9716,31 +10151,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="833" t="s">
+      <c r="C6" s="978" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="844" t="s">
+      <c r="D6" s="989" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="855" t="s">
+      <c r="E6" s="1000" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="865" t="s">
+      <c r="F6" s="1010" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="876" t="s">
+      <c r="G6" s="1021" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="887" t="s">
+      <c r="H6" s="1032" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="898" t="s">
+      <c r="I6" s="1043" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="909" t="s">
+      <c r="J6" s="1054" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="920" t="s">
+      <c r="K6" s="1065" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="9"/>
@@ -9754,29 +10189,29 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="834" t="s">
+      <c r="C7" s="979" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="845" t="s">
+      <c r="D7" s="990" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="866" t="s">
+      <c r="F7" s="1011" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="877" t="s">
+      <c r="G7" s="1022" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="888" t="s">
+      <c r="H7" s="1033" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="899" t="s">
+      <c r="I7" s="1044" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="910" t="s">
+      <c r="J7" s="1055" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="921" t="s">
+      <c r="K7" s="1066" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="9"/>
@@ -9790,31 +10225,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="835" t="s">
+      <c r="C8" s="980" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="846" t="s">
+      <c r="D8" s="991" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="856" t="s">
+      <c r="E8" s="1001" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="867" t="s">
+      <c r="F8" s="1012" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="878" t="s">
+      <c r="G8" s="1023" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="889" t="s">
+      <c r="H8" s="1034" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="900" t="s">
+      <c r="I8" s="1045" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="911" t="s">
+      <c r="J8" s="1056" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="922" t="s">
+      <c r="K8" s="1067" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="9"/>
@@ -9828,31 +10263,31 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="836" t="s">
+      <c r="C9" s="981" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="847" t="s">
+      <c r="D9" s="992" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="857" t="s">
+      <c r="E9" s="1002" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="868" t="s">
+      <c r="F9" s="1013" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="879" t="s">
+      <c r="G9" s="1024" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="890" t="s">
+      <c r="H9" s="1035" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="901" t="s">
+      <c r="I9" s="1046" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="912" t="s">
+      <c r="J9" s="1057" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="923" t="s">
+      <c r="K9" s="1068" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="9"/>
@@ -9866,31 +10301,31 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="837" t="s">
+      <c r="C10" s="982" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="848" t="s">
+      <c r="D10" s="993" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="858" t="s">
+      <c r="E10" s="1003" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="869" t="s">
+      <c r="F10" s="1014" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="880" t="s">
+      <c r="G10" s="1025" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="891" t="s">
+      <c r="H10" s="1036" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="902" t="s">
+      <c r="I10" s="1047" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="913" t="s">
+      <c r="J10" s="1058" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="924" t="s">
+      <c r="K10" s="1069" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="9"/>
@@ -9904,31 +10339,31 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="838" t="s">
+      <c r="C11" s="983" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="849" t="s">
+      <c r="D11" s="994" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="859" t="s">
+      <c r="E11" s="1004" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="870" t="s">
+      <c r="F11" s="1015" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="881" t="s">
+      <c r="G11" s="1026" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="892" t="s">
+      <c r="H11" s="1037" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="903" t="s">
+      <c r="I11" s="1048" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="914" t="s">
+      <c r="J11" s="1059" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="925" t="s">
+      <c r="K11" s="1070" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="9"/>
@@ -9942,31 +10377,31 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="839" t="s">
+      <c r="C12" s="984" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="850" t="s">
+      <c r="D12" s="995" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="860" t="s">
+      <c r="E12" s="1005" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="871" t="s">
+      <c r="F12" s="1016" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="882" t="s">
+      <c r="G12" s="1027" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="893" t="s">
+      <c r="H12" s="1038" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="904" t="s">
+      <c r="I12" s="1049" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="915" t="s">
+      <c r="J12" s="1060" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="926" t="s">
+      <c r="K12" s="1071" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="9"/>
@@ -9980,31 +10415,31 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="840" t="s">
+      <c r="C13" s="985" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="851" t="s">
+      <c r="D13" s="996" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="861" t="s">
+      <c r="E13" s="1006" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="872" t="s">
+      <c r="F13" s="1017" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="883" t="s">
+      <c r="G13" s="1028" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="894" t="s">
+      <c r="H13" s="1039" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="905" t="s">
+      <c r="I13" s="1050" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="916" t="s">
+      <c r="J13" s="1061" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="927" t="s">
+      <c r="K13" s="1072" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="9"/>

</xml_diff>

<commit_message>
fingers crossed it doesn't delete femalesSing
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="172">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -896,7 +896,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1073">
+  <cellXfs count="1218">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1001,6 +1001,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -7200,42 +7635,42 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="928" t="s">
+      <c r="A3" s="1073" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="930" t="s">
+      <c r="B3" s="1075" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="932" t="s">
+      <c r="C3" s="1077" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="934" t="s">
+      <c r="D3" s="1079" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="936" t="s">
+      <c r="E3" s="1081" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="938" t="s">
+      <c r="F3" s="1083" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="929" t="s">
+      <c r="A4" s="1074" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="931" t="s">
+      <c r="B4" s="1076" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="933" t="s">
+      <c r="C4" s="1078" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="935" t="s">
+      <c r="D4" s="1080" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="937" t="s">
+      <c r="E4" s="1082" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="939" t="s">
+      <c r="F4" s="1084" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8389,25 +8824,25 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="940" t="s">
+      <c r="C3" s="1085" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="945" t="s">
+      <c r="D3" s="1090" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="950" t="s">
+      <c r="E3" s="1095" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="955" t="s">
+      <c r="F3" s="1100" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="960" t="s">
+      <c r="G3" s="1105" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="965" t="s">
+      <c r="H3" s="1110" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="970" t="s">
+      <c r="I3" s="1115" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -8415,25 +8850,25 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="941" t="s">
+      <c r="C4" s="1086" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="946" t="s">
+      <c r="D4" s="1091" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="951" t="s">
+      <c r="E4" s="1096" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="956" t="s">
+      <c r="F4" s="1101" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="961" t="s">
+      <c r="G4" s="1106" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="966" t="s">
+      <c r="H4" s="1111" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="971" t="s">
+      <c r="I4" s="1116" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -8441,25 +8876,25 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="942" t="s">
+      <c r="C5" s="1087" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="947" t="s">
+      <c r="D5" s="1092" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="952" t="s">
+      <c r="E5" s="1097" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="957" t="s">
+      <c r="F5" s="1102" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="962" t="s">
+      <c r="G5" s="1107" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="967" t="s">
+      <c r="H5" s="1112" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="972" t="s">
+      <c r="I5" s="1117" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -8467,25 +8902,25 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="943" t="s">
+      <c r="C6" s="1088" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="948" t="s">
+      <c r="D6" s="1093" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="953" t="s">
+      <c r="E6" s="1098" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="958" t="s">
+      <c r="F6" s="1103" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="963" t="s">
+      <c r="G6" s="1108" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="968" t="s">
+      <c r="H6" s="1113" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="973" t="s">
+      <c r="I6" s="1118" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -8493,25 +8928,25 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="944" t="s">
+      <c r="C7" s="1089" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="949" t="s">
+      <c r="D7" s="1094" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="954" t="s">
+      <c r="E7" s="1099" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="959" t="s">
+      <c r="F7" s="1104" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="964" t="s">
+      <c r="G7" s="1109" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="969" t="s">
+      <c r="H7" s="1114" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="974" t="s">
+      <c r="I7" s="1119" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -10037,31 +10472,31 @@
     <row r="3">
       <c r="A3" s="24"/>
       <c r="B3"/>
-      <c r="C3" s="975" t="s">
+      <c r="C3" s="1120" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="986" t="s">
+      <c r="D3" s="1131" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="997" t="s">
+      <c r="E3" s="1142" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="1007" t="s">
+      <c r="F3" s="1152" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="1018" t="s">
+      <c r="G3" s="1163" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="1029" t="s">
+      <c r="H3" s="1174" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="1040" t="s">
+      <c r="I3" s="1185" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="1051" t="s">
+      <c r="J3" s="1196" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="1062" t="s">
+      <c r="K3" s="1207" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="9"/>
@@ -10075,31 +10510,31 @@
     <row r="4">
       <c r="A4" s="24"/>
       <c r="B4"/>
-      <c r="C4" s="976" t="s">
+      <c r="C4" s="1121" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="987" t="s">
+      <c r="D4" s="1132" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="998" t="s">
+      <c r="E4" s="1143" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="1008" t="s">
+      <c r="F4" s="1153" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="1019" t="s">
+      <c r="G4" s="1164" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="1030" t="s">
+      <c r="H4" s="1175" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="1041" t="s">
+      <c r="I4" s="1186" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="1052" t="s">
+      <c r="J4" s="1197" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="1063" t="s">
+      <c r="K4" s="1208" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="9"/>
@@ -10113,31 +10548,31 @@
     <row r="5">
       <c r="A5" s="24"/>
       <c r="B5"/>
-      <c r="C5" s="977" t="s">
+      <c r="C5" s="1122" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="988" t="s">
+      <c r="D5" s="1133" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="999" t="s">
+      <c r="E5" s="1144" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="1009" t="s">
+      <c r="F5" s="1154" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="1020" t="s">
+      <c r="G5" s="1165" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="1031" t="s">
+      <c r="H5" s="1176" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="1042" t="s">
+      <c r="I5" s="1187" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="1053" t="s">
+      <c r="J5" s="1198" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="1064" t="s">
+      <c r="K5" s="1209" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="9"/>
@@ -10151,31 +10586,31 @@
     <row r="6">
       <c r="A6" s="24"/>
       <c r="B6"/>
-      <c r="C6" s="978" t="s">
+      <c r="C6" s="1123" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="989" t="s">
+      <c r="D6" s="1134" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="1000" t="s">
+      <c r="E6" s="1145" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="1010" t="s">
+      <c r="F6" s="1155" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="1021" t="s">
+      <c r="G6" s="1166" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="1032" t="s">
+      <c r="H6" s="1177" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="1043" t="s">
+      <c r="I6" s="1188" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="1054" t="s">
+      <c r="J6" s="1199" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="1065" t="s">
+      <c r="K6" s="1210" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="9"/>
@@ -10189,29 +10624,29 @@
     <row r="7">
       <c r="A7" s="24"/>
       <c r="B7"/>
-      <c r="C7" s="979" t="s">
+      <c r="C7" s="1124" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="990" t="s">
+      <c r="D7" s="1135" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="1011" t="s">
+      <c r="F7" s="1156" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="1022" t="s">
+      <c r="G7" s="1167" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="1033" t="s">
+      <c r="H7" s="1178" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="1044" t="s">
+      <c r="I7" s="1189" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="1055" t="s">
+      <c r="J7" s="1200" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="1066" t="s">
+      <c r="K7" s="1211" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="9"/>
@@ -10225,31 +10660,31 @@
     <row r="8">
       <c r="A8" s="24"/>
       <c r="B8"/>
-      <c r="C8" s="980" t="s">
+      <c r="C8" s="1125" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="991" t="s">
+      <c r="D8" s="1136" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="1001" t="s">
+      <c r="E8" s="1146" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="1012" t="s">
+      <c r="F8" s="1157" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="1023" t="s">
+      <c r="G8" s="1168" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="1034" t="s">
+      <c r="H8" s="1179" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="1045" t="s">
+      <c r="I8" s="1190" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="1056" t="s">
+      <c r="J8" s="1201" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="1067" t="s">
+      <c r="K8" s="1212" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="9"/>
@@ -10263,31 +10698,31 @@
     <row r="9">
       <c r="A9" s="24"/>
       <c r="B9"/>
-      <c r="C9" s="981" t="s">
+      <c r="C9" s="1126" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="992" t="s">
+      <c r="D9" s="1137" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="1002" t="s">
+      <c r="E9" s="1147" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="1013" t="s">
+      <c r="F9" s="1158" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="1024" t="s">
+      <c r="G9" s="1169" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="1035" t="s">
+      <c r="H9" s="1180" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="1046" t="s">
+      <c r="I9" s="1191" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="1057" t="s">
+      <c r="J9" s="1202" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="1068" t="s">
+      <c r="K9" s="1213" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="9"/>
@@ -10301,31 +10736,31 @@
     <row r="10">
       <c r="A10" s="24"/>
       <c r="B10"/>
-      <c r="C10" s="982" t="s">
+      <c r="C10" s="1127" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="993" t="s">
+      <c r="D10" s="1138" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1003" t="s">
+      <c r="E10" s="1148" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="1014" t="s">
+      <c r="F10" s="1159" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1025" t="s">
+      <c r="G10" s="1170" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1036" t="s">
+      <c r="H10" s="1181" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="1047" t="s">
+      <c r="I10" s="1192" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="1058" t="s">
+      <c r="J10" s="1203" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1069" t="s">
+      <c r="K10" s="1214" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="9"/>
@@ -10339,31 +10774,31 @@
     <row r="11">
       <c r="A11" s="24"/>
       <c r="B11"/>
-      <c r="C11" s="983" t="s">
+      <c r="C11" s="1128" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="994" t="s">
+      <c r="D11" s="1139" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1004" t="s">
+      <c r="E11" s="1149" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="1015" t="s">
+      <c r="F11" s="1160" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="1026" t="s">
+      <c r="G11" s="1171" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="1037" t="s">
+      <c r="H11" s="1182" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="1048" t="s">
+      <c r="I11" s="1193" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="1059" t="s">
+      <c r="J11" s="1204" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="1070" t="s">
+      <c r="K11" s="1215" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="9"/>
@@ -10377,31 +10812,31 @@
     <row r="12">
       <c r="A12" s="24"/>
       <c r="B12"/>
-      <c r="C12" s="984" t="s">
+      <c r="C12" s="1129" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="995" t="s">
+      <c r="D12" s="1140" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="1005" t="s">
+      <c r="E12" s="1150" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="1016" t="s">
+      <c r="F12" s="1161" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="1027" t="s">
+      <c r="G12" s="1172" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="1038" t="s">
+      <c r="H12" s="1183" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="1049" t="s">
+      <c r="I12" s="1194" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="1060" t="s">
+      <c r="J12" s="1205" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="1071" t="s">
+      <c r="K12" s="1216" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="9"/>
@@ -10415,31 +10850,31 @@
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13"/>
-      <c r="C13" s="985" t="s">
+      <c r="C13" s="1130" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="996" t="s">
+      <c r="D13" s="1141" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="1006" t="s">
+      <c r="E13" s="1151" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="1017" t="s">
+      <c r="F13" s="1162" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="1028" t="s">
+      <c r="G13" s="1173" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="1039" t="s">
+      <c r="H13" s="1184" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="1050" t="s">
+      <c r="I13" s="1195" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="1061" t="s">
+      <c r="J13" s="1206" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="1072" t="s">
+      <c r="K13" s="1217" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="9"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-03 18:12:35]  updating background finally
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="179">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="354">
+  <cellXfs count="934">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1053,6 +1053,1746 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -5077,42 +6817,42 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="209" t="s">
+      <c r="A3" s="789" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="211" t="s">
+      <c r="B3" s="791" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="213" t="s">
+      <c r="C3" s="793" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="215" t="s">
+      <c r="D3" s="795" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="217" t="s">
+      <c r="E3" s="797" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="219" t="s">
+      <c r="F3" s="799" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="210" t="s">
+      <c r="A4" s="790" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="212" t="s">
+      <c r="B4" s="792" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="214" t="s">
+      <c r="C4" s="794" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="216" t="s">
+      <c r="D4" s="796" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="218" t="s">
+      <c r="E4" s="798" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="220" t="s">
+      <c r="F4" s="800" t="s">
         <v>34</v>
       </c>
     </row>
@@ -6266,25 +8006,25 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="221" t="s">
+      <c r="C3" s="801" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="226" t="s">
+      <c r="D3" s="806" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="231" t="s">
+      <c r="E3" s="811" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="236" t="s">
+      <c r="F3" s="816" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="241" t="s">
+      <c r="G3" s="821" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="246" t="s">
+      <c r="H3" s="826" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="251" t="s">
+      <c r="I3" s="831" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -6292,25 +8032,25 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="222" t="s">
+      <c r="C4" s="802" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="227" t="s">
+      <c r="D4" s="807" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="232" t="s">
+      <c r="E4" s="812" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="237" t="s">
+      <c r="F4" s="817" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="242" t="s">
+      <c r="G4" s="822" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="247" t="s">
+      <c r="H4" s="827" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="252" t="s">
+      <c r="I4" s="832" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -6318,25 +8058,25 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="803" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="228" t="s">
+      <c r="D5" s="808" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="233" t="s">
+      <c r="E5" s="813" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="238" t="s">
+      <c r="F5" s="818" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="243" t="s">
+      <c r="G5" s="823" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="248" t="s">
+      <c r="H5" s="828" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="253" t="s">
+      <c r="I5" s="833" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -6344,25 +8084,25 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="224" t="s">
+      <c r="C6" s="804" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="229" t="s">
+      <c r="D6" s="809" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="234" t="s">
+      <c r="E6" s="814" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="239" t="s">
+      <c r="F6" s="819" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="244" t="s">
+      <c r="G6" s="824" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="249" t="s">
+      <c r="H6" s="829" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="254" t="s">
+      <c r="I6" s="834" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -6370,25 +8110,25 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="225" t="s">
+      <c r="C7" s="805" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="230" t="s">
+      <c r="D7" s="810" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="235" t="s">
+      <c r="E7" s="815" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="240" t="s">
+      <c r="F7" s="820" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="245" t="s">
+      <c r="G7" s="825" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="250" t="s">
+      <c r="H7" s="830" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="255" t="s">
+      <c r="I7" s="835" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -7914,31 +9654,31 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="256" t="s">
+      <c r="C3" s="836" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="267" t="s">
+      <c r="D3" s="847" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="278" t="s">
+      <c r="E3" s="858" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="288" t="s">
+      <c r="F3" s="868" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="299" t="s">
+      <c r="G3" s="879" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="310" t="s">
+      <c r="H3" s="890" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="321" t="s">
+      <c r="I3" s="901" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="332" t="s">
+      <c r="J3" s="912" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="343" t="s">
+      <c r="K3" s="923" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="8"/>
@@ -7952,31 +9692,31 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="257" t="s">
+      <c r="C4" s="837" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="268" t="s">
+      <c r="D4" s="848" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="279" t="s">
+      <c r="E4" s="859" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="289" t="s">
+      <c r="F4" s="869" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="300" t="s">
+      <c r="G4" s="880" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="311" t="s">
+      <c r="H4" s="891" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="322" t="s">
+      <c r="I4" s="902" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="333" t="s">
+      <c r="J4" s="913" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="344" t="s">
+      <c r="K4" s="924" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="8"/>
@@ -7990,31 +9730,31 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="258" t="s">
+      <c r="C5" s="838" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="269" t="s">
+      <c r="D5" s="849" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="280" t="s">
+      <c r="E5" s="860" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="290" t="s">
+      <c r="F5" s="870" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="301" t="s">
+      <c r="G5" s="881" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="312" t="s">
+      <c r="H5" s="892" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="323" t="s">
+      <c r="I5" s="903" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="334" t="s">
+      <c r="J5" s="914" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="345" t="s">
+      <c r="K5" s="925" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="8"/>
@@ -8028,31 +9768,31 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="259" t="s">
+      <c r="C6" s="839" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="270" t="s">
+      <c r="D6" s="850" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="281" t="s">
+      <c r="E6" s="861" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="291" t="s">
+      <c r="F6" s="871" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="302" t="s">
+      <c r="G6" s="882" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="313" t="s">
+      <c r="H6" s="893" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="324" t="s">
+      <c r="I6" s="904" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="335" t="s">
+      <c r="J6" s="915" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="346" t="s">
+      <c r="K6" s="926" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="8"/>
@@ -8066,29 +9806,29 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="260" t="s">
+      <c r="C7" s="840" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="271" t="s">
+      <c r="D7" s="851" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="292" t="s">
+      <c r="F7" s="872" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="303" t="s">
+      <c r="G7" s="883" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="314" t="s">
+      <c r="H7" s="894" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="325" t="s">
+      <c r="I7" s="905" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="336" t="s">
+      <c r="J7" s="916" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="347" t="s">
+      <c r="K7" s="927" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="8"/>
@@ -8102,31 +9842,31 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="261" t="s">
+      <c r="C8" s="841" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="272" t="s">
+      <c r="D8" s="852" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="282" t="s">
+      <c r="E8" s="862" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="293" t="s">
+      <c r="F8" s="873" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="304" t="s">
+      <c r="G8" s="884" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="315" t="s">
+      <c r="H8" s="895" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="326" t="s">
+      <c r="I8" s="906" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="337" t="s">
+      <c r="J8" s="917" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="348" t="s">
+      <c r="K8" s="928" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="8"/>
@@ -8140,31 +9880,31 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="262" t="s">
+      <c r="C9" s="842" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="273" t="s">
+      <c r="D9" s="853" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="283" t="s">
+      <c r="E9" s="863" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="294" t="s">
+      <c r="F9" s="874" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="305" t="s">
+      <c r="G9" s="885" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="316" t="s">
+      <c r="H9" s="896" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="327" t="s">
+      <c r="I9" s="907" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="338" t="s">
+      <c r="J9" s="918" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="349" t="s">
+      <c r="K9" s="929" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -8178,31 +9918,31 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="263" t="s">
+      <c r="C10" s="843" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="274" t="s">
+      <c r="D10" s="854" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="284" t="s">
+      <c r="E10" s="864" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="295" t="s">
+      <c r="F10" s="875" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="306" t="s">
+      <c r="G10" s="886" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="317" t="s">
+      <c r="H10" s="897" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="328" t="s">
+      <c r="I10" s="908" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="339" t="s">
+      <c r="J10" s="919" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="350" t="s">
+      <c r="K10" s="930" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="8"/>
@@ -8216,31 +9956,31 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="264" t="s">
+      <c r="C11" s="844" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="275" t="s">
+      <c r="D11" s="855" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="285" t="s">
+      <c r="E11" s="865" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="296" t="s">
+      <c r="F11" s="876" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="307" t="s">
+      <c r="G11" s="887" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="318" t="s">
+      <c r="H11" s="898" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="329" t="s">
+      <c r="I11" s="909" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="340" t="s">
+      <c r="J11" s="920" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="351" t="s">
+      <c r="K11" s="931" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="8"/>
@@ -8254,31 +9994,31 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="265" t="s">
+      <c r="C12" s="845" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="276" t="s">
+      <c r="D12" s="856" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="286" t="s">
+      <c r="E12" s="866" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="297" t="s">
+      <c r="F12" s="877" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="308" t="s">
+      <c r="G12" s="888" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="319" t="s">
+      <c r="H12" s="899" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="330" t="s">
+      <c r="I12" s="910" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="341" t="s">
+      <c r="J12" s="921" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="352" t="s">
+      <c r="K12" s="932" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="8"/>
@@ -8292,31 +10032,31 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="266" t="s">
+      <c r="C13" s="846" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="277" t="s">
+      <c r="D13" s="857" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="287" t="s">
+      <c r="E13" s="867" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="298" t="s">
+      <c r="F13" s="878" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="309" t="s">
+      <c r="G13" s="889" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="320" t="s">
+      <c r="H13" s="900" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="331" t="s">
+      <c r="I13" s="911" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="342" t="s">
+      <c r="J13" s="922" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="353" t="s">
+      <c r="K13" s="933" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-03 18:27:59]  trying again with background
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="179">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="934">
+  <cellXfs count="1079">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1053,6 +1053,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -6817,42 +7252,42 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="789" t="s">
+      <c r="A3" s="934" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="791" t="s">
+      <c r="B3" s="936" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="793" t="s">
+      <c r="C3" s="938" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="795" t="s">
+      <c r="D3" s="940" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="797" t="s">
+      <c r="E3" s="942" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="799" t="s">
+      <c r="F3" s="944" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="790" t="s">
+      <c r="A4" s="935" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="792" t="s">
+      <c r="B4" s="937" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="794" t="s">
+      <c r="C4" s="939" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="796" t="s">
+      <c r="D4" s="941" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="798" t="s">
+      <c r="E4" s="943" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="800" t="s">
+      <c r="F4" s="945" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8006,25 +8441,25 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="801" t="s">
+      <c r="C3" s="946" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="806" t="s">
+      <c r="D3" s="951" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="811" t="s">
+      <c r="E3" s="956" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="816" t="s">
+      <c r="F3" s="961" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="821" t="s">
+      <c r="G3" s="966" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="826" t="s">
+      <c r="H3" s="971" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="831" t="s">
+      <c r="I3" s="976" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -8032,25 +8467,25 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="802" t="s">
+      <c r="C4" s="947" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="807" t="s">
+      <c r="D4" s="952" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="812" t="s">
+      <c r="E4" s="957" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="817" t="s">
+      <c r="F4" s="962" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="822" t="s">
+      <c r="G4" s="967" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="827" t="s">
+      <c r="H4" s="972" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="832" t="s">
+      <c r="I4" s="977" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -8058,25 +8493,25 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="803" t="s">
+      <c r="C5" s="948" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="808" t="s">
+      <c r="D5" s="953" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="813" t="s">
+      <c r="E5" s="958" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="818" t="s">
+      <c r="F5" s="963" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="823" t="s">
+      <c r="G5" s="968" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="828" t="s">
+      <c r="H5" s="973" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="833" t="s">
+      <c r="I5" s="978" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -8084,25 +8519,25 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="804" t="s">
+      <c r="C6" s="949" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="809" t="s">
+      <c r="D6" s="954" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="814" t="s">
+      <c r="E6" s="959" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="819" t="s">
+      <c r="F6" s="964" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="824" t="s">
+      <c r="G6" s="969" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="829" t="s">
+      <c r="H6" s="974" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="834" t="s">
+      <c r="I6" s="979" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -8110,25 +8545,25 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="805" t="s">
+      <c r="C7" s="950" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="810" t="s">
+      <c r="D7" s="955" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="815" t="s">
+      <c r="E7" s="960" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="820" t="s">
+      <c r="F7" s="965" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="825" t="s">
+      <c r="G7" s="970" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="830" t="s">
+      <c r="H7" s="975" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="835" t="s">
+      <c r="I7" s="980" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -9654,31 +10089,31 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="836" t="s">
+      <c r="C3" s="981" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="847" t="s">
+      <c r="D3" s="992" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="858" t="s">
+      <c r="E3" s="1003" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="868" t="s">
+      <c r="F3" s="1013" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="879" t="s">
+      <c r="G3" s="1024" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="890" t="s">
+      <c r="H3" s="1035" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="901" t="s">
+      <c r="I3" s="1046" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="912" t="s">
+      <c r="J3" s="1057" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="923" t="s">
+      <c r="K3" s="1068" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="8"/>
@@ -9692,31 +10127,31 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="837" t="s">
+      <c r="C4" s="982" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="848" t="s">
+      <c r="D4" s="993" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="859" t="s">
+      <c r="E4" s="1004" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="869" t="s">
+      <c r="F4" s="1014" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="880" t="s">
+      <c r="G4" s="1025" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="891" t="s">
+      <c r="H4" s="1036" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="902" t="s">
+      <c r="I4" s="1047" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="913" t="s">
+      <c r="J4" s="1058" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="924" t="s">
+      <c r="K4" s="1069" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="8"/>
@@ -9730,31 +10165,31 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="838" t="s">
+      <c r="C5" s="983" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="849" t="s">
+      <c r="D5" s="994" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="860" t="s">
+      <c r="E5" s="1005" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="870" t="s">
+      <c r="F5" s="1015" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="881" t="s">
+      <c r="G5" s="1026" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="892" t="s">
+      <c r="H5" s="1037" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="903" t="s">
+      <c r="I5" s="1048" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="914" t="s">
+      <c r="J5" s="1059" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="925" t="s">
+      <c r="K5" s="1070" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="8"/>
@@ -9768,31 +10203,31 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="839" t="s">
+      <c r="C6" s="984" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="850" t="s">
+      <c r="D6" s="995" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="861" t="s">
+      <c r="E6" s="1006" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="871" t="s">
+      <c r="F6" s="1016" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="882" t="s">
+      <c r="G6" s="1027" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="893" t="s">
+      <c r="H6" s="1038" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="904" t="s">
+      <c r="I6" s="1049" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="915" t="s">
+      <c r="J6" s="1060" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="926" t="s">
+      <c r="K6" s="1071" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="8"/>
@@ -9806,29 +10241,29 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="840" t="s">
+      <c r="C7" s="985" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="851" t="s">
+      <c r="D7" s="996" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="872" t="s">
+      <c r="F7" s="1017" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="883" t="s">
+      <c r="G7" s="1028" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="894" t="s">
+      <c r="H7" s="1039" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="905" t="s">
+      <c r="I7" s="1050" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="916" t="s">
+      <c r="J7" s="1061" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="927" t="s">
+      <c r="K7" s="1072" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="8"/>
@@ -9842,31 +10277,31 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="841" t="s">
+      <c r="C8" s="986" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="852" t="s">
+      <c r="D8" s="997" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="862" t="s">
+      <c r="E8" s="1007" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="873" t="s">
+      <c r="F8" s="1018" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="884" t="s">
+      <c r="G8" s="1029" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="895" t="s">
+      <c r="H8" s="1040" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="906" t="s">
+      <c r="I8" s="1051" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="917" t="s">
+      <c r="J8" s="1062" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="928" t="s">
+      <c r="K8" s="1073" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="8"/>
@@ -9880,31 +10315,31 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="842" t="s">
+      <c r="C9" s="987" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="853" t="s">
+      <c r="D9" s="998" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="863" t="s">
+      <c r="E9" s="1008" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="874" t="s">
+      <c r="F9" s="1019" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="885" t="s">
+      <c r="G9" s="1030" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="896" t="s">
+      <c r="H9" s="1041" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="907" t="s">
+      <c r="I9" s="1052" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="918" t="s">
+      <c r="J9" s="1063" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="929" t="s">
+      <c r="K9" s="1074" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -9918,31 +10353,31 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="843" t="s">
+      <c r="C10" s="988" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="854" t="s">
+      <c r="D10" s="999" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="864" t="s">
+      <c r="E10" s="1009" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="875" t="s">
+      <c r="F10" s="1020" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="886" t="s">
+      <c r="G10" s="1031" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="897" t="s">
+      <c r="H10" s="1042" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="908" t="s">
+      <c r="I10" s="1053" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="919" t="s">
+      <c r="J10" s="1064" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="930" t="s">
+      <c r="K10" s="1075" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="8"/>
@@ -9956,31 +10391,31 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="844" t="s">
+      <c r="C11" s="989" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="855" t="s">
+      <c r="D11" s="1000" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="865" t="s">
+      <c r="E11" s="1010" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="876" t="s">
+      <c r="F11" s="1021" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="887" t="s">
+      <c r="G11" s="1032" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="898" t="s">
+      <c r="H11" s="1043" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="909" t="s">
+      <c r="I11" s="1054" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="920" t="s">
+      <c r="J11" s="1065" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="931" t="s">
+      <c r="K11" s="1076" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="8"/>
@@ -9994,31 +10429,31 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="845" t="s">
+      <c r="C12" s="990" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="856" t="s">
+      <c r="D12" s="1001" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="866" t="s">
+      <c r="E12" s="1011" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="877" t="s">
+      <c r="F12" s="1022" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="888" t="s">
+      <c r="G12" s="1033" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="899" t="s">
+      <c r="H12" s="1044" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="910" t="s">
+      <c r="I12" s="1055" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="921" t="s">
+      <c r="J12" s="1066" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="932" t="s">
+      <c r="K12" s="1077" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="8"/>
@@ -10032,31 +10467,31 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="846" t="s">
+      <c r="C13" s="991" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="857" t="s">
+      <c r="D13" s="1002" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="867" t="s">
+      <c r="E13" s="1012" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="878" t="s">
+      <c r="F13" s="1023" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="889" t="s">
+      <c r="G13" s="1034" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="900" t="s">
+      <c r="H13" s="1045" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="911" t="s">
+      <c r="I13" s="1056" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="922" t="s">
+      <c r="J13" s="1067" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="933" t="s">
+      <c r="K13" s="1078" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-03 18:33:47]  try again
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="179">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1079">
+  <cellXfs count="1224">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1053,6 +1053,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -7252,42 +7687,42 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="934" t="s">
+      <c r="A3" s="1079" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="936" t="s">
+      <c r="B3" s="1081" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="938" t="s">
+      <c r="C3" s="1083" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="940" t="s">
+      <c r="D3" s="1085" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="942" t="s">
+      <c r="E3" s="1087" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="944" t="s">
+      <c r="F3" s="1089" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="935" t="s">
+      <c r="A4" s="1080" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="937" t="s">
+      <c r="B4" s="1082" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="939" t="s">
+      <c r="C4" s="1084" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="941" t="s">
+      <c r="D4" s="1086" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="943" t="s">
+      <c r="E4" s="1088" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="945" t="s">
+      <c r="F4" s="1090" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8441,25 +8876,25 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="946" t="s">
+      <c r="C3" s="1091" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="951" t="s">
+      <c r="D3" s="1096" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="956" t="s">
+      <c r="E3" s="1101" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="961" t="s">
+      <c r="F3" s="1106" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="966" t="s">
+      <c r="G3" s="1111" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="971" t="s">
+      <c r="H3" s="1116" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="976" t="s">
+      <c r="I3" s="1121" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -8467,25 +8902,25 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="947" t="s">
+      <c r="C4" s="1092" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="952" t="s">
+      <c r="D4" s="1097" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="957" t="s">
+      <c r="E4" s="1102" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="962" t="s">
+      <c r="F4" s="1107" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="967" t="s">
+      <c r="G4" s="1112" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="972" t="s">
+      <c r="H4" s="1117" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="977" t="s">
+      <c r="I4" s="1122" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -8493,25 +8928,25 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="948" t="s">
+      <c r="C5" s="1093" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="953" t="s">
+      <c r="D5" s="1098" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="958" t="s">
+      <c r="E5" s="1103" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="963" t="s">
+      <c r="F5" s="1108" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="968" t="s">
+      <c r="G5" s="1113" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="973" t="s">
+      <c r="H5" s="1118" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="978" t="s">
+      <c r="I5" s="1123" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -8519,25 +8954,25 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="949" t="s">
+      <c r="C6" s="1094" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="954" t="s">
+      <c r="D6" s="1099" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="959" t="s">
+      <c r="E6" s="1104" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="964" t="s">
+      <c r="F6" s="1109" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="969" t="s">
+      <c r="G6" s="1114" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="974" t="s">
+      <c r="H6" s="1119" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="979" t="s">
+      <c r="I6" s="1124" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -8545,25 +8980,25 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="950" t="s">
+      <c r="C7" s="1095" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="955" t="s">
+      <c r="D7" s="1100" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="960" t="s">
+      <c r="E7" s="1105" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="965" t="s">
+      <c r="F7" s="1110" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="970" t="s">
+      <c r="G7" s="1115" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="975" t="s">
+      <c r="H7" s="1120" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="980" t="s">
+      <c r="I7" s="1125" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -10089,31 +10524,31 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="981" t="s">
+      <c r="C3" s="1126" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="992" t="s">
+      <c r="D3" s="1137" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1003" t="s">
+      <c r="E3" s="1148" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="1013" t="s">
+      <c r="F3" s="1158" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="1024" t="s">
+      <c r="G3" s="1169" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="1035" t="s">
+      <c r="H3" s="1180" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="1046" t="s">
+      <c r="I3" s="1191" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="1057" t="s">
+      <c r="J3" s="1202" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="1068" t="s">
+      <c r="K3" s="1213" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="8"/>
@@ -10127,31 +10562,31 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="982" t="s">
+      <c r="C4" s="1127" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="993" t="s">
+      <c r="D4" s="1138" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="1004" t="s">
+      <c r="E4" s="1149" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="1014" t="s">
+      <c r="F4" s="1159" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="1025" t="s">
+      <c r="G4" s="1170" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="1036" t="s">
+      <c r="H4" s="1181" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="1047" t="s">
+      <c r="I4" s="1192" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="1058" t="s">
+      <c r="J4" s="1203" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="1069" t="s">
+      <c r="K4" s="1214" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="8"/>
@@ -10165,31 +10600,31 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="983" t="s">
+      <c r="C5" s="1128" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="994" t="s">
+      <c r="D5" s="1139" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="1005" t="s">
+      <c r="E5" s="1150" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="1015" t="s">
+      <c r="F5" s="1160" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="1026" t="s">
+      <c r="G5" s="1171" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="1037" t="s">
+      <c r="H5" s="1182" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="1048" t="s">
+      <c r="I5" s="1193" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="1059" t="s">
+      <c r="J5" s="1204" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="1070" t="s">
+      <c r="K5" s="1215" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="8"/>
@@ -10203,31 +10638,31 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="984" t="s">
+      <c r="C6" s="1129" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="995" t="s">
+      <c r="D6" s="1140" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="1006" t="s">
+      <c r="E6" s="1151" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="1016" t="s">
+      <c r="F6" s="1161" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="1027" t="s">
+      <c r="G6" s="1172" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="1038" t="s">
+      <c r="H6" s="1183" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="1049" t="s">
+      <c r="I6" s="1194" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="1060" t="s">
+      <c r="J6" s="1205" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="1071" t="s">
+      <c r="K6" s="1216" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="8"/>
@@ -10241,29 +10676,29 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="985" t="s">
+      <c r="C7" s="1130" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="996" t="s">
+      <c r="D7" s="1141" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="1017" t="s">
+      <c r="F7" s="1162" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="1028" t="s">
+      <c r="G7" s="1173" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="1039" t="s">
+      <c r="H7" s="1184" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="1050" t="s">
+      <c r="I7" s="1195" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="1061" t="s">
+      <c r="J7" s="1206" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="1072" t="s">
+      <c r="K7" s="1217" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="8"/>
@@ -10277,31 +10712,31 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="986" t="s">
+      <c r="C8" s="1131" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="997" t="s">
+      <c r="D8" s="1142" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="1007" t="s">
+      <c r="E8" s="1152" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="1018" t="s">
+      <c r="F8" s="1163" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="1029" t="s">
+      <c r="G8" s="1174" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="1040" t="s">
+      <c r="H8" s="1185" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="1051" t="s">
+      <c r="I8" s="1196" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="1062" t="s">
+      <c r="J8" s="1207" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="1073" t="s">
+      <c r="K8" s="1218" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="8"/>
@@ -10315,31 +10750,31 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="987" t="s">
+      <c r="C9" s="1132" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="998" t="s">
+      <c r="D9" s="1143" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="1008" t="s">
+      <c r="E9" s="1153" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="1019" t="s">
+      <c r="F9" s="1164" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="1030" t="s">
+      <c r="G9" s="1175" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="1041" t="s">
+      <c r="H9" s="1186" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="1052" t="s">
+      <c r="I9" s="1197" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="1063" t="s">
+      <c r="J9" s="1208" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="1074" t="s">
+      <c r="K9" s="1219" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -10353,31 +10788,31 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="988" t="s">
+      <c r="C10" s="1133" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="999" t="s">
+      <c r="D10" s="1144" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1009" t="s">
+      <c r="E10" s="1154" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="1020" t="s">
+      <c r="F10" s="1165" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1031" t="s">
+      <c r="G10" s="1176" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1042" t="s">
+      <c r="H10" s="1187" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="1053" t="s">
+      <c r="I10" s="1198" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="1064" t="s">
+      <c r="J10" s="1209" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1075" t="s">
+      <c r="K10" s="1220" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="8"/>
@@ -10391,31 +10826,31 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="989" t="s">
+      <c r="C11" s="1134" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1000" t="s">
+      <c r="D11" s="1145" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1010" t="s">
+      <c r="E11" s="1155" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="1021" t="s">
+      <c r="F11" s="1166" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="1032" t="s">
+      <c r="G11" s="1177" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="1043" t="s">
+      <c r="H11" s="1188" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="1054" t="s">
+      <c r="I11" s="1199" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="1065" t="s">
+      <c r="J11" s="1210" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="1076" t="s">
+      <c r="K11" s="1221" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="8"/>
@@ -10429,31 +10864,31 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="990" t="s">
+      <c r="C12" s="1135" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1001" t="s">
+      <c r="D12" s="1146" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="1011" t="s">
+      <c r="E12" s="1156" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="1022" t="s">
+      <c r="F12" s="1167" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="1033" t="s">
+      <c r="G12" s="1178" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="1044" t="s">
+      <c r="H12" s="1189" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="1055" t="s">
+      <c r="I12" s="1200" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="1066" t="s">
+      <c r="J12" s="1211" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="1077" t="s">
+      <c r="K12" s="1222" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="8"/>
@@ -10467,31 +10902,31 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="991" t="s">
+      <c r="C13" s="1136" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1002" t="s">
+      <c r="D13" s="1147" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="1012" t="s">
+      <c r="E13" s="1157" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="1023" t="s">
+      <c r="F13" s="1168" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="1034" t="s">
+      <c r="G13" s="1179" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="1045" t="s">
+      <c r="H13" s="1190" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="1056" t="s">
+      <c r="I13" s="1201" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="1067" t="s">
+      <c r="J13" s="1212" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="1078" t="s">
+      <c r="K13" s="1223" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-03 21:55:02]  acknowledgments and whatnot
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="179">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1369">
+  <cellXfs count="1514">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1053,6 +1053,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -8122,42 +8557,42 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1224" t="s">
+      <c r="A3" s="1369" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1226" t="s">
+      <c r="B3" s="1371" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1228" t="s">
+      <c r="C3" s="1373" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1230" t="s">
+      <c r="D3" s="1375" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1232" t="s">
+      <c r="E3" s="1377" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="1234" t="s">
+      <c r="F3" s="1379" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1225" t="s">
+      <c r="A4" s="1370" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1227" t="s">
+      <c r="B4" s="1372" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1229" t="s">
+      <c r="C4" s="1374" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1231" t="s">
+      <c r="D4" s="1376" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1233" t="s">
+      <c r="E4" s="1378" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="1235" t="s">
+      <c r="F4" s="1380" t="s">
         <v>34</v>
       </c>
     </row>
@@ -9311,25 +9746,25 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="1236" t="s">
+      <c r="C3" s="1381" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1241" t="s">
+      <c r="D3" s="1386" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1246" t="s">
+      <c r="E3" s="1391" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="1251" t="s">
+      <c r="F3" s="1396" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="1256" t="s">
+      <c r="G3" s="1401" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="1261" t="s">
+      <c r="H3" s="1406" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1266" t="s">
+      <c r="I3" s="1411" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -9337,25 +9772,25 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="1237" t="s">
+      <c r="C4" s="1382" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1242" t="s">
+      <c r="D4" s="1387" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="1247" t="s">
+      <c r="E4" s="1392" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="1252" t="s">
+      <c r="F4" s="1397" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="1257" t="s">
+      <c r="G4" s="1402" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="1262" t="s">
+      <c r="H4" s="1407" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="1267" t="s">
+      <c r="I4" s="1412" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -9363,25 +9798,25 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="1238" t="s">
+      <c r="C5" s="1383" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1243" t="s">
+      <c r="D5" s="1388" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="1248" t="s">
+      <c r="E5" s="1393" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="1253" t="s">
+      <c r="F5" s="1398" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="1258" t="s">
+      <c r="G5" s="1403" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="1263" t="s">
+      <c r="H5" s="1408" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="1268" t="s">
+      <c r="I5" s="1413" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -9389,25 +9824,25 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="1239" t="s">
+      <c r="C6" s="1384" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1244" t="s">
+      <c r="D6" s="1389" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="1249" t="s">
+      <c r="E6" s="1394" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="1254" t="s">
+      <c r="F6" s="1399" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="1259" t="s">
+      <c r="G6" s="1404" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1264" t="s">
+      <c r="H6" s="1409" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="1269" t="s">
+      <c r="I6" s="1414" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -9415,25 +9850,25 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="1240" t="s">
+      <c r="C7" s="1385" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1245" t="s">
+      <c r="D7" s="1390" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="1250" t="s">
+      <c r="E7" s="1395" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="1255" t="s">
+      <c r="F7" s="1400" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="1260" t="s">
+      <c r="G7" s="1405" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1265" t="s">
+      <c r="H7" s="1410" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="1270" t="s">
+      <c r="I7" s="1415" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -10959,31 +11394,31 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="1271" t="s">
+      <c r="C3" s="1416" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1282" t="s">
+      <c r="D3" s="1427" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1293" t="s">
+      <c r="E3" s="1438" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="1303" t="s">
+      <c r="F3" s="1448" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="1314" t="s">
+      <c r="G3" s="1459" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="1325" t="s">
+      <c r="H3" s="1470" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="1336" t="s">
+      <c r="I3" s="1481" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="1347" t="s">
+      <c r="J3" s="1492" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="1358" t="s">
+      <c r="K3" s="1503" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="8"/>
@@ -10997,31 +11432,31 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="1272" t="s">
+      <c r="C4" s="1417" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1283" t="s">
+      <c r="D4" s="1428" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="1294" t="s">
+      <c r="E4" s="1439" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="1304" t="s">
+      <c r="F4" s="1449" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="1315" t="s">
+      <c r="G4" s="1460" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="1326" t="s">
+      <c r="H4" s="1471" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="1337" t="s">
+      <c r="I4" s="1482" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="1348" t="s">
+      <c r="J4" s="1493" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="1359" t="s">
+      <c r="K4" s="1504" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="8"/>
@@ -11035,31 +11470,31 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="1273" t="s">
+      <c r="C5" s="1418" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1284" t="s">
+      <c r="D5" s="1429" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="1295" t="s">
+      <c r="E5" s="1440" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="1305" t="s">
+      <c r="F5" s="1450" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="1316" t="s">
+      <c r="G5" s="1461" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="1327" t="s">
+      <c r="H5" s="1472" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="1338" t="s">
+      <c r="I5" s="1483" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="1349" t="s">
+      <c r="J5" s="1494" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="1360" t="s">
+      <c r="K5" s="1505" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="8"/>
@@ -11073,31 +11508,31 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="1274" t="s">
+      <c r="C6" s="1419" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1285" t="s">
+      <c r="D6" s="1430" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="1296" t="s">
+      <c r="E6" s="1441" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="1306" t="s">
+      <c r="F6" s="1451" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="1317" t="s">
+      <c r="G6" s="1462" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="1328" t="s">
+      <c r="H6" s="1473" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="1339" t="s">
+      <c r="I6" s="1484" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="1350" t="s">
+      <c r="J6" s="1495" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="1361" t="s">
+      <c r="K6" s="1506" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="8"/>
@@ -11111,29 +11546,29 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="1275" t="s">
+      <c r="C7" s="1420" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1286" t="s">
+      <c r="D7" s="1431" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="1307" t="s">
+      <c r="F7" s="1452" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="1318" t="s">
+      <c r="G7" s="1463" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="1329" t="s">
+      <c r="H7" s="1474" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="1340" t="s">
+      <c r="I7" s="1485" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="1351" t="s">
+      <c r="J7" s="1496" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="1362" t="s">
+      <c r="K7" s="1507" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="8"/>
@@ -11147,31 +11582,31 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="1276" t="s">
+      <c r="C8" s="1421" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1287" t="s">
+      <c r="D8" s="1432" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="1297" t="s">
+      <c r="E8" s="1442" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="1308" t="s">
+      <c r="F8" s="1453" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="1319" t="s">
+      <c r="G8" s="1464" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="1330" t="s">
+      <c r="H8" s="1475" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="1341" t="s">
+      <c r="I8" s="1486" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="1352" t="s">
+      <c r="J8" s="1497" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="1363" t="s">
+      <c r="K8" s="1508" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="8"/>
@@ -11185,31 +11620,31 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="1277" t="s">
+      <c r="C9" s="1422" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1288" t="s">
+      <c r="D9" s="1433" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="1298" t="s">
+      <c r="E9" s="1443" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="1309" t="s">
+      <c r="F9" s="1454" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="1320" t="s">
+      <c r="G9" s="1465" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="1331" t="s">
+      <c r="H9" s="1476" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="1342" t="s">
+      <c r="I9" s="1487" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="1353" t="s">
+      <c r="J9" s="1498" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="1364" t="s">
+      <c r="K9" s="1509" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -11223,31 +11658,31 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="1278" t="s">
+      <c r="C10" s="1423" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1289" t="s">
+      <c r="D10" s="1434" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1299" t="s">
+      <c r="E10" s="1444" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="1310" t="s">
+      <c r="F10" s="1455" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1321" t="s">
+      <c r="G10" s="1466" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1332" t="s">
+      <c r="H10" s="1477" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="1343" t="s">
+      <c r="I10" s="1488" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="1354" t="s">
+      <c r="J10" s="1499" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1365" t="s">
+      <c r="K10" s="1510" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="8"/>
@@ -11261,31 +11696,31 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="1279" t="s">
+      <c r="C11" s="1424" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1290" t="s">
+      <c r="D11" s="1435" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1300" t="s">
+      <c r="E11" s="1445" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="1311" t="s">
+      <c r="F11" s="1456" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="1322" t="s">
+      <c r="G11" s="1467" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="1333" t="s">
+      <c r="H11" s="1478" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="1344" t="s">
+      <c r="I11" s="1489" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="1355" t="s">
+      <c r="J11" s="1500" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="1366" t="s">
+      <c r="K11" s="1511" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="8"/>
@@ -11299,31 +11734,31 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="1280" t="s">
+      <c r="C12" s="1425" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1291" t="s">
+      <c r="D12" s="1436" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="1301" t="s">
+      <c r="E12" s="1446" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="1312" t="s">
+      <c r="F12" s="1457" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="1323" t="s">
+      <c r="G12" s="1468" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="1334" t="s">
+      <c r="H12" s="1479" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="1345" t="s">
+      <c r="I12" s="1490" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="1356" t="s">
+      <c r="J12" s="1501" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="1367" t="s">
+      <c r="K12" s="1512" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="8"/>
@@ -11337,31 +11772,31 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="1281" t="s">
+      <c r="C13" s="1426" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1292" t="s">
+      <c r="D13" s="1437" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="1302" t="s">
+      <c r="E13" s="1447" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="1313" t="s">
+      <c r="F13" s="1458" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="1324" t="s">
+      <c r="G13" s="1469" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="1335" t="s">
+      <c r="H13" s="1480" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="1346" t="s">
+      <c r="I13" s="1491" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="1357" t="s">
+      <c r="J13" s="1502" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="1368" t="s">
+      <c r="K13" s="1513" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-03 23:03:59]  fix duplicated thumbnail study pics
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="179">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1659">
+  <cellXfs count="2094">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1053,6 +1053,1311 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -8992,42 +10297,42 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1514" t="s">
+      <c r="A3" s="1949" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1516" t="s">
+      <c r="B3" s="1951" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1518" t="s">
+      <c r="C3" s="1953" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1520" t="s">
+      <c r="D3" s="1955" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1522" t="s">
+      <c r="E3" s="1957" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="1524" t="s">
+      <c r="F3" s="1959" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1515" t="s">
+      <c r="A4" s="1950" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1517" t="s">
+      <c r="B4" s="1952" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1519" t="s">
+      <c r="C4" s="1954" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1521" t="s">
+      <c r="D4" s="1956" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1523" t="s">
+      <c r="E4" s="1958" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="1525" t="s">
+      <c r="F4" s="1960" t="s">
         <v>34</v>
       </c>
     </row>
@@ -10181,25 +11486,25 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="1526" t="s">
+      <c r="C3" s="1961" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1531" t="s">
+      <c r="D3" s="1966" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1536" t="s">
+      <c r="E3" s="1971" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="1541" t="s">
+      <c r="F3" s="1976" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="1546" t="s">
+      <c r="G3" s="1981" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="1551" t="s">
+      <c r="H3" s="1986" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1556" t="s">
+      <c r="I3" s="1991" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -10207,25 +11512,25 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="1527" t="s">
+      <c r="C4" s="1962" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1532" t="s">
+      <c r="D4" s="1967" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="1537" t="s">
+      <c r="E4" s="1972" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="1542" t="s">
+      <c r="F4" s="1977" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="1547" t="s">
+      <c r="G4" s="1982" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="1552" t="s">
+      <c r="H4" s="1987" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="1557" t="s">
+      <c r="I4" s="1992" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -10233,25 +11538,25 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="1528" t="s">
+      <c r="C5" s="1963" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1533" t="s">
+      <c r="D5" s="1968" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="1538" t="s">
+      <c r="E5" s="1973" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="1543" t="s">
+      <c r="F5" s="1978" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="1548" t="s">
+      <c r="G5" s="1983" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="1553" t="s">
+      <c r="H5" s="1988" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="1558" t="s">
+      <c r="I5" s="1993" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -10259,25 +11564,25 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="1529" t="s">
+      <c r="C6" s="1964" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1534" t="s">
+      <c r="D6" s="1969" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="1539" t="s">
+      <c r="E6" s="1974" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="1544" t="s">
+      <c r="F6" s="1979" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="1549" t="s">
+      <c r="G6" s="1984" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1554" t="s">
+      <c r="H6" s="1989" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="1559" t="s">
+      <c r="I6" s="1994" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -10285,25 +11590,25 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="1530" t="s">
+      <c r="C7" s="1965" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1535" t="s">
+      <c r="D7" s="1970" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="1540" t="s">
+      <c r="E7" s="1975" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="1545" t="s">
+      <c r="F7" s="1980" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="1550" t="s">
+      <c r="G7" s="1985" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1555" t="s">
+      <c r="H7" s="1990" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="1560" t="s">
+      <c r="I7" s="1995" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -11829,31 +13134,31 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="1561" t="s">
+      <c r="C3" s="1996" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1572" t="s">
+      <c r="D3" s="2007" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1583" t="s">
+      <c r="E3" s="2018" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="1593" t="s">
+      <c r="F3" s="2028" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="1604" t="s">
+      <c r="G3" s="2039" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="1615" t="s">
+      <c r="H3" s="2050" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="1626" t="s">
+      <c r="I3" s="2061" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="1637" t="s">
+      <c r="J3" s="2072" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="1648" t="s">
+      <c r="K3" s="2083" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="8"/>
@@ -11867,31 +13172,31 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="1562" t="s">
+      <c r="C4" s="1997" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1573" t="s">
+      <c r="D4" s="2008" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="1584" t="s">
+      <c r="E4" s="2019" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="1594" t="s">
+      <c r="F4" s="2029" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="1605" t="s">
+      <c r="G4" s="2040" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="1616" t="s">
+      <c r="H4" s="2051" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="1627" t="s">
+      <c r="I4" s="2062" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="1638" t="s">
+      <c r="J4" s="2073" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="1649" t="s">
+      <c r="K4" s="2084" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="8"/>
@@ -11905,31 +13210,31 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="1563" t="s">
+      <c r="C5" s="1998" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1574" t="s">
+      <c r="D5" s="2009" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="1585" t="s">
+      <c r="E5" s="2020" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="1595" t="s">
+      <c r="F5" s="2030" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="1606" t="s">
+      <c r="G5" s="2041" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="1617" t="s">
+      <c r="H5" s="2052" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="1628" t="s">
+      <c r="I5" s="2063" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="1639" t="s">
+      <c r="J5" s="2074" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="1650" t="s">
+      <c r="K5" s="2085" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="8"/>
@@ -11943,31 +13248,31 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="1564" t="s">
+      <c r="C6" s="1999" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1575" t="s">
+      <c r="D6" s="2010" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="1586" t="s">
+      <c r="E6" s="2021" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="1596" t="s">
+      <c r="F6" s="2031" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="1607" t="s">
+      <c r="G6" s="2042" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="1618" t="s">
+      <c r="H6" s="2053" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="1629" t="s">
+      <c r="I6" s="2064" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="1640" t="s">
+      <c r="J6" s="2075" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="1651" t="s">
+      <c r="K6" s="2086" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="8"/>
@@ -11981,29 +13286,29 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="1565" t="s">
+      <c r="C7" s="2000" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1576" t="s">
+      <c r="D7" s="2011" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="1597" t="s">
+      <c r="F7" s="2032" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="1608" t="s">
+      <c r="G7" s="2043" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="1619" t="s">
+      <c r="H7" s="2054" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="1630" t="s">
+      <c r="I7" s="2065" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="1641" t="s">
+      <c r="J7" s="2076" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="1652" t="s">
+      <c r="K7" s="2087" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="8"/>
@@ -12017,31 +13322,31 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="1566" t="s">
+      <c r="C8" s="2001" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1577" t="s">
+      <c r="D8" s="2012" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="1587" t="s">
+      <c r="E8" s="2022" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="1598" t="s">
+      <c r="F8" s="2033" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="1609" t="s">
+      <c r="G8" s="2044" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="1620" t="s">
+      <c r="H8" s="2055" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="1631" t="s">
+      <c r="I8" s="2066" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="1642" t="s">
+      <c r="J8" s="2077" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="1653" t="s">
+      <c r="K8" s="2088" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="8"/>
@@ -12055,31 +13360,31 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="1567" t="s">
+      <c r="C9" s="2002" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1578" t="s">
+      <c r="D9" s="2013" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="1588" t="s">
+      <c r="E9" s="2023" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="1599" t="s">
+      <c r="F9" s="2034" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="1610" t="s">
+      <c r="G9" s="2045" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="1621" t="s">
+      <c r="H9" s="2056" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="1632" t="s">
+      <c r="I9" s="2067" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="1643" t="s">
+      <c r="J9" s="2078" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="1654" t="s">
+      <c r="K9" s="2089" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -12093,31 +13398,31 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="1568" t="s">
+      <c r="C10" s="2003" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1579" t="s">
+      <c r="D10" s="2014" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1589" t="s">
+      <c r="E10" s="2024" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="1600" t="s">
+      <c r="F10" s="2035" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1611" t="s">
+      <c r="G10" s="2046" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1622" t="s">
+      <c r="H10" s="2057" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="1633" t="s">
+      <c r="I10" s="2068" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="1644" t="s">
+      <c r="J10" s="2079" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1655" t="s">
+      <c r="K10" s="2090" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="8"/>
@@ -12131,31 +13436,31 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="1569" t="s">
+      <c r="C11" s="2004" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1580" t="s">
+      <c r="D11" s="2015" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1590" t="s">
+      <c r="E11" s="2025" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="1601" t="s">
+      <c r="F11" s="2036" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="1612" t="s">
+      <c r="G11" s="2047" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="1623" t="s">
+      <c r="H11" s="2058" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="1634" t="s">
+      <c r="I11" s="2069" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="1645" t="s">
+      <c r="J11" s="2080" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="1656" t="s">
+      <c r="K11" s="2091" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="8"/>
@@ -12169,31 +13474,31 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="1570" t="s">
+      <c r="C12" s="2005" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1581" t="s">
+      <c r="D12" s="2016" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="1591" t="s">
+      <c r="E12" s="2026" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="1602" t="s">
+      <c r="F12" s="2037" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="1613" t="s">
+      <c r="G12" s="2048" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="1624" t="s">
+      <c r="H12" s="2059" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="1635" t="s">
+      <c r="I12" s="2070" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="1646" t="s">
+      <c r="J12" s="2081" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="1657" t="s">
+      <c r="K12" s="2092" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="8"/>
@@ -12207,31 +13512,31 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="1571" t="s">
+      <c r="C13" s="2006" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1582" t="s">
+      <c r="D13" s="2017" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="1592" t="s">
+      <c r="E13" s="2027" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="1603" t="s">
+      <c r="F13" s="2038" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="1614" t="s">
+      <c r="G13" s="2049" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="1625" t="s">
+      <c r="H13" s="2060" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="1636" t="s">
+      <c r="I13" s="2071" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="1647" t="s">
+      <c r="J13" s="2082" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="1658" t="s">
+      <c r="K13" s="2093" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-03 23:11:56]  simplified paper link
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2612" uniqueCount="179">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2094">
+  <cellXfs count="2239">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1053,6 +1053,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -10297,42 +10732,42 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1949" t="s">
+      <c r="A3" s="2094" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1951" t="s">
+      <c r="B3" s="2096" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1953" t="s">
+      <c r="C3" s="2098" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1955" t="s">
+      <c r="D3" s="2100" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1957" t="s">
+      <c r="E3" s="2102" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="1959" t="s">
+      <c r="F3" s="2104" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1950" t="s">
+      <c r="A4" s="2095" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1952" t="s">
+      <c r="B4" s="2097" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1954" t="s">
+      <c r="C4" s="2099" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1956" t="s">
+      <c r="D4" s="2101" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1958" t="s">
+      <c r="E4" s="2103" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="1960" t="s">
+      <c r="F4" s="2105" t="s">
         <v>34</v>
       </c>
     </row>
@@ -11486,25 +11921,25 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="1961" t="s">
+      <c r="C3" s="2106" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1966" t="s">
+      <c r="D3" s="2111" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1971" t="s">
+      <c r="E3" s="2116" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="1976" t="s">
+      <c r="F3" s="2121" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="1981" t="s">
+      <c r="G3" s="2126" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="1986" t="s">
+      <c r="H3" s="2131" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1991" t="s">
+      <c r="I3" s="2136" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -11512,25 +11947,25 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="1962" t="s">
+      <c r="C4" s="2107" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1967" t="s">
+      <c r="D4" s="2112" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="1972" t="s">
+      <c r="E4" s="2117" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="1977" t="s">
+      <c r="F4" s="2122" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="1982" t="s">
+      <c r="G4" s="2127" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="1987" t="s">
+      <c r="H4" s="2132" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="1992" t="s">
+      <c r="I4" s="2137" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -11538,25 +11973,25 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="1963" t="s">
+      <c r="C5" s="2108" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1968" t="s">
+      <c r="D5" s="2113" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="1973" t="s">
+      <c r="E5" s="2118" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="1978" t="s">
+      <c r="F5" s="2123" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="1983" t="s">
+      <c r="G5" s="2128" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="1988" t="s">
+      <c r="H5" s="2133" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="1993" t="s">
+      <c r="I5" s="2138" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -11564,25 +11999,25 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="1964" t="s">
+      <c r="C6" s="2109" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1969" t="s">
+      <c r="D6" s="2114" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="1974" t="s">
+      <c r="E6" s="2119" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="1979" t="s">
+      <c r="F6" s="2124" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="1984" t="s">
+      <c r="G6" s="2129" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1989" t="s">
+      <c r="H6" s="2134" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="1994" t="s">
+      <c r="I6" s="2139" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -11590,25 +12025,25 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="1965" t="s">
+      <c r="C7" s="2110" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1970" t="s">
+      <c r="D7" s="2115" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="1975" t="s">
+      <c r="E7" s="2120" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="1980" t="s">
+      <c r="F7" s="2125" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="1985" t="s">
+      <c r="G7" s="2130" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1990" t="s">
+      <c r="H7" s="2135" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="1995" t="s">
+      <c r="I7" s="2140" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -13134,31 +13569,31 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="1996" t="s">
+      <c r="C3" s="2141" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2007" t="s">
+      <c r="D3" s="2152" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="2018" t="s">
+      <c r="E3" s="2163" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="2028" t="s">
+      <c r="F3" s="2173" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="2039" t="s">
+      <c r="G3" s="2184" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="2050" t="s">
+      <c r="H3" s="2195" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="2061" t="s">
+      <c r="I3" s="2206" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="2072" t="s">
+      <c r="J3" s="2217" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="2083" t="s">
+      <c r="K3" s="2228" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="8"/>
@@ -13172,31 +13607,31 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="1997" t="s">
+      <c r="C4" s="2142" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2008" t="s">
+      <c r="D4" s="2153" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="2019" t="s">
+      <c r="E4" s="2164" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="2029" t="s">
+      <c r="F4" s="2174" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="2040" t="s">
+      <c r="G4" s="2185" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="2051" t="s">
+      <c r="H4" s="2196" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="2062" t="s">
+      <c r="I4" s="2207" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="2073" t="s">
+      <c r="J4" s="2218" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="2084" t="s">
+      <c r="K4" s="2229" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="8"/>
@@ -13210,31 +13645,31 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="1998" t="s">
+      <c r="C5" s="2143" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2009" t="s">
+      <c r="D5" s="2154" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="2020" t="s">
+      <c r="E5" s="2165" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="2030" t="s">
+      <c r="F5" s="2175" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="2041" t="s">
+      <c r="G5" s="2186" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="2052" t="s">
+      <c r="H5" s="2197" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="2063" t="s">
+      <c r="I5" s="2208" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="2074" t="s">
+      <c r="J5" s="2219" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="2085" t="s">
+      <c r="K5" s="2230" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="8"/>
@@ -13248,31 +13683,31 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="1999" t="s">
+      <c r="C6" s="2144" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2010" t="s">
+      <c r="D6" s="2155" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="2021" t="s">
+      <c r="E6" s="2166" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="2031" t="s">
+      <c r="F6" s="2176" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="2042" t="s">
+      <c r="G6" s="2187" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="2053" t="s">
+      <c r="H6" s="2198" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="2064" t="s">
+      <c r="I6" s="2209" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="2075" t="s">
+      <c r="J6" s="2220" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="2086" t="s">
+      <c r="K6" s="2231" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="8"/>
@@ -13286,29 +13721,29 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="2000" t="s">
+      <c r="C7" s="2145" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2011" t="s">
+      <c r="D7" s="2156" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="2032" t="s">
+      <c r="F7" s="2177" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="2043" t="s">
+      <c r="G7" s="2188" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="2054" t="s">
+      <c r="H7" s="2199" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="2065" t="s">
+      <c r="I7" s="2210" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="2076" t="s">
+      <c r="J7" s="2221" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="2087" t="s">
+      <c r="K7" s="2232" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="8"/>
@@ -13322,31 +13757,31 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="2001" t="s">
+      <c r="C8" s="2146" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2012" t="s">
+      <c r="D8" s="2157" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="2022" t="s">
+      <c r="E8" s="2167" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="2033" t="s">
+      <c r="F8" s="2178" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="2044" t="s">
+      <c r="G8" s="2189" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="2055" t="s">
+      <c r="H8" s="2200" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="2066" t="s">
+      <c r="I8" s="2211" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="2077" t="s">
+      <c r="J8" s="2222" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="2088" t="s">
+      <c r="K8" s="2233" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="8"/>
@@ -13360,31 +13795,31 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="2002" t="s">
+      <c r="C9" s="2147" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2013" t="s">
+      <c r="D9" s="2158" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="2023" t="s">
+      <c r="E9" s="2168" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="2034" t="s">
+      <c r="F9" s="2179" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="2045" t="s">
+      <c r="G9" s="2190" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="2056" t="s">
+      <c r="H9" s="2201" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="2067" t="s">
+      <c r="I9" s="2212" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="2078" t="s">
+      <c r="J9" s="2223" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="2089" t="s">
+      <c r="K9" s="2234" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -13398,31 +13833,31 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="2003" t="s">
+      <c r="C10" s="2148" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2014" t="s">
+      <c r="D10" s="2159" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="2024" t="s">
+      <c r="E10" s="2169" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="2035" t="s">
+      <c r="F10" s="2180" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2046" t="s">
+      <c r="G10" s="2191" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="2057" t="s">
+      <c r="H10" s="2202" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="2068" t="s">
+      <c r="I10" s="2213" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="2079" t="s">
+      <c r="J10" s="2224" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="2090" t="s">
+      <c r="K10" s="2235" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="8"/>
@@ -13436,31 +13871,31 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="2004" t="s">
+      <c r="C11" s="2149" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2015" t="s">
+      <c r="D11" s="2160" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2025" t="s">
+      <c r="E11" s="2170" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="2036" t="s">
+      <c r="F11" s="2181" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="2047" t="s">
+      <c r="G11" s="2192" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="2058" t="s">
+      <c r="H11" s="2203" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="2069" t="s">
+      <c r="I11" s="2214" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="2080" t="s">
+      <c r="J11" s="2225" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="2091" t="s">
+      <c r="K11" s="2236" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="8"/>
@@ -13474,31 +13909,31 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="2005" t="s">
+      <c r="C12" s="2150" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2016" t="s">
+      <c r="D12" s="2161" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="2026" t="s">
+      <c r="E12" s="2171" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="2037" t="s">
+      <c r="F12" s="2182" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="2048" t="s">
+      <c r="G12" s="2193" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="2059" t="s">
+      <c r="H12" s="2204" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="2070" t="s">
+      <c r="I12" s="2215" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="2081" t="s">
+      <c r="J12" s="2226" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="2092" t="s">
+      <c r="K12" s="2237" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="8"/>
@@ -13512,31 +13947,31 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="2006" t="s">
+      <c r="C13" s="2151" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="2017" t="s">
+      <c r="D13" s="2162" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="2027" t="s">
+      <c r="E13" s="2172" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="2038" t="s">
+      <c r="F13" s="2183" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="2049" t="s">
+      <c r="G13" s="2194" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="2060" t="s">
+      <c r="H13" s="2205" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="2071" t="s">
+      <c r="I13" s="2216" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="2082" t="s">
+      <c r="J13" s="2227" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="2093" t="s">
+      <c r="K13" s="2238" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-08 16:02:52]  updating feedback links
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2902" uniqueCount="179">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2384">
+  <cellXfs count="2529">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1053,6 +1053,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -11167,42 +11602,42 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="2239" t="s">
+      <c r="A3" s="2384" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2241" t="s">
+      <c r="B3" s="2386" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2243" t="s">
+      <c r="C3" s="2388" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2245" t="s">
+      <c r="D3" s="2390" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="2247" t="s">
+      <c r="E3" s="2392" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2249" t="s">
+      <c r="F3" s="2394" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2240" t="s">
+      <c r="A4" s="2385" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2242" t="s">
+      <c r="B4" s="2387" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2244" t="s">
+      <c r="C4" s="2389" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2246" t="s">
+      <c r="D4" s="2391" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2248" t="s">
+      <c r="E4" s="2393" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="2250" t="s">
+      <c r="F4" s="2395" t="s">
         <v>34</v>
       </c>
     </row>
@@ -12356,25 +12791,25 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="2251" t="s">
+      <c r="C3" s="2396" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2256" t="s">
+      <c r="D3" s="2401" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="2261" t="s">
+      <c r="E3" s="2406" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="2266" t="s">
+      <c r="F3" s="2411" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="2271" t="s">
+      <c r="G3" s="2416" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="2276" t="s">
+      <c r="H3" s="2421" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="2281" t="s">
+      <c r="I3" s="2426" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -12382,25 +12817,25 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="2252" t="s">
+      <c r="C4" s="2397" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2257" t="s">
+      <c r="D4" s="2402" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="2262" t="s">
+      <c r="E4" s="2407" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="2267" t="s">
+      <c r="F4" s="2412" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="2272" t="s">
+      <c r="G4" s="2417" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="2277" t="s">
+      <c r="H4" s="2422" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="2282" t="s">
+      <c r="I4" s="2427" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -12408,25 +12843,25 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="2253" t="s">
+      <c r="C5" s="2398" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2258" t="s">
+      <c r="D5" s="2403" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="2263" t="s">
+      <c r="E5" s="2408" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="2268" t="s">
+      <c r="F5" s="2413" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="2273" t="s">
+      <c r="G5" s="2418" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="2278" t="s">
+      <c r="H5" s="2423" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="2283" t="s">
+      <c r="I5" s="2428" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -12434,25 +12869,25 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="2254" t="s">
+      <c r="C6" s="2399" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2259" t="s">
+      <c r="D6" s="2404" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="2264" t="s">
+      <c r="E6" s="2409" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="2269" t="s">
+      <c r="F6" s="2414" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="2274" t="s">
+      <c r="G6" s="2419" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="2279" t="s">
+      <c r="H6" s="2424" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="2284" t="s">
+      <c r="I6" s="2429" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -12460,25 +12895,25 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="2255" t="s">
+      <c r="C7" s="2400" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2260" t="s">
+      <c r="D7" s="2405" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="2265" t="s">
+      <c r="E7" s="2410" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="2270" t="s">
+      <c r="F7" s="2415" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="2275" t="s">
+      <c r="G7" s="2420" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="2280" t="s">
+      <c r="H7" s="2425" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="2285" t="s">
+      <c r="I7" s="2430" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -14004,31 +14439,31 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="2286" t="s">
+      <c r="C3" s="2431" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2297" t="s">
+      <c r="D3" s="2442" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="2308" t="s">
+      <c r="E3" s="2453" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="2318" t="s">
+      <c r="F3" s="2463" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="2329" t="s">
+      <c r="G3" s="2474" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="2340" t="s">
+      <c r="H3" s="2485" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="2351" t="s">
+      <c r="I3" s="2496" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="2362" t="s">
+      <c r="J3" s="2507" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="2373" t="s">
+      <c r="K3" s="2518" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="8"/>
@@ -14042,31 +14477,31 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="2287" t="s">
+      <c r="C4" s="2432" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2298" t="s">
+      <c r="D4" s="2443" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="2309" t="s">
+      <c r="E4" s="2454" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="2319" t="s">
+      <c r="F4" s="2464" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="2330" t="s">
+      <c r="G4" s="2475" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="2341" t="s">
+      <c r="H4" s="2486" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="2352" t="s">
+      <c r="I4" s="2497" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="2363" t="s">
+      <c r="J4" s="2508" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="2374" t="s">
+      <c r="K4" s="2519" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="8"/>
@@ -14080,31 +14515,31 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="2288" t="s">
+      <c r="C5" s="2433" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2299" t="s">
+      <c r="D5" s="2444" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="2310" t="s">
+      <c r="E5" s="2455" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="2320" t="s">
+      <c r="F5" s="2465" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="2331" t="s">
+      <c r="G5" s="2476" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="2342" t="s">
+      <c r="H5" s="2487" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="2353" t="s">
+      <c r="I5" s="2498" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="2364" t="s">
+      <c r="J5" s="2509" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="2375" t="s">
+      <c r="K5" s="2520" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="8"/>
@@ -14118,31 +14553,31 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="2289" t="s">
+      <c r="C6" s="2434" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2300" t="s">
+      <c r="D6" s="2445" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="2311" t="s">
+      <c r="E6" s="2456" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="2321" t="s">
+      <c r="F6" s="2466" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="2332" t="s">
+      <c r="G6" s="2477" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="2343" t="s">
+      <c r="H6" s="2488" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="2354" t="s">
+      <c r="I6" s="2499" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="2365" t="s">
+      <c r="J6" s="2510" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="2376" t="s">
+      <c r="K6" s="2521" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="8"/>
@@ -14156,29 +14591,29 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="2290" t="s">
+      <c r="C7" s="2435" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2301" t="s">
+      <c r="D7" s="2446" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="2322" t="s">
+      <c r="F7" s="2467" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="2333" t="s">
+      <c r="G7" s="2478" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="2344" t="s">
+      <c r="H7" s="2489" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="2355" t="s">
+      <c r="I7" s="2500" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="2366" t="s">
+      <c r="J7" s="2511" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="2377" t="s">
+      <c r="K7" s="2522" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="8"/>
@@ -14192,31 +14627,31 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="2291" t="s">
+      <c r="C8" s="2436" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2302" t="s">
+      <c r="D8" s="2447" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="2312" t="s">
+      <c r="E8" s="2457" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="2323" t="s">
+      <c r="F8" s="2468" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="2334" t="s">
+      <c r="G8" s="2479" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="2345" t="s">
+      <c r="H8" s="2490" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="2356" t="s">
+      <c r="I8" s="2501" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="2367" t="s">
+      <c r="J8" s="2512" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="2378" t="s">
+      <c r="K8" s="2523" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="8"/>
@@ -14230,31 +14665,31 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="2292" t="s">
+      <c r="C9" s="2437" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2303" t="s">
+      <c r="D9" s="2448" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="2313" t="s">
+      <c r="E9" s="2458" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="2324" t="s">
+      <c r="F9" s="2469" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="2335" t="s">
+      <c r="G9" s="2480" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="2346" t="s">
+      <c r="H9" s="2491" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="2357" t="s">
+      <c r="I9" s="2502" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="2368" t="s">
+      <c r="J9" s="2513" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="2379" t="s">
+      <c r="K9" s="2524" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -14268,31 +14703,31 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="2293" t="s">
+      <c r="C10" s="2438" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2304" t="s">
+      <c r="D10" s="2449" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="2314" t="s">
+      <c r="E10" s="2459" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="2325" t="s">
+      <c r="F10" s="2470" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2336" t="s">
+      <c r="G10" s="2481" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="2347" t="s">
+      <c r="H10" s="2492" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="2358" t="s">
+      <c r="I10" s="2503" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="2369" t="s">
+      <c r="J10" s="2514" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="2380" t="s">
+      <c r="K10" s="2525" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="8"/>
@@ -14306,31 +14741,31 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="2294" t="s">
+      <c r="C11" s="2439" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2305" t="s">
+      <c r="D11" s="2450" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2315" t="s">
+      <c r="E11" s="2460" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="2326" t="s">
+      <c r="F11" s="2471" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="2337" t="s">
+      <c r="G11" s="2482" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="2348" t="s">
+      <c r="H11" s="2493" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="2359" t="s">
+      <c r="I11" s="2504" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="2370" t="s">
+      <c r="J11" s="2515" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="2381" t="s">
+      <c r="K11" s="2526" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="8"/>
@@ -14344,31 +14779,31 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="2295" t="s">
+      <c r="C12" s="2440" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2306" t="s">
+      <c r="D12" s="2451" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="2316" t="s">
+      <c r="E12" s="2461" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="2327" t="s">
+      <c r="F12" s="2472" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="2338" t="s">
+      <c r="G12" s="2483" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="2349" t="s">
+      <c r="H12" s="2494" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="2360" t="s">
+      <c r="I12" s="2505" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="2371" t="s">
+      <c r="J12" s="2516" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="2382" t="s">
+      <c r="K12" s="2527" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="8"/>
@@ -14382,31 +14817,31 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="2296" t="s">
+      <c r="C13" s="2441" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="2307" t="s">
+      <c r="D13" s="2452" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="2317" t="s">
+      <c r="E13" s="2462" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="2328" t="s">
+      <c r="F13" s="2473" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="2339" t="s">
+      <c r="G13" s="2484" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="2350" t="s">
+      <c r="H13" s="2495" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="2361" t="s">
+      <c r="I13" s="2506" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="2372" t="s">
+      <c r="J13" s="2517" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="2383" t="s">
+      <c r="K13" s="2528" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-03-08 21:52:17]  typo
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2902" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3047" uniqueCount="179">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2529">
+  <cellXfs count="2674">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1053,6 +1053,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -11602,42 +12037,42 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="2384" t="s">
+      <c r="A3" s="2529" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2386" t="s">
+      <c r="B3" s="2531" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2388" t="s">
+      <c r="C3" s="2533" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2390" t="s">
+      <c r="D3" s="2535" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="2392" t="s">
+      <c r="E3" s="2537" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2394" t="s">
+      <c r="F3" s="2539" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2385" t="s">
+      <c r="A4" s="2530" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2387" t="s">
+      <c r="B4" s="2532" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2389" t="s">
+      <c r="C4" s="2534" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2391" t="s">
+      <c r="D4" s="2536" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2393" t="s">
+      <c r="E4" s="2538" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="2395" t="s">
+      <c r="F4" s="2540" t="s">
         <v>34</v>
       </c>
     </row>
@@ -12791,25 +13226,25 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="2396" t="s">
+      <c r="C3" s="2541" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2401" t="s">
+      <c r="D3" s="2546" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="2406" t="s">
+      <c r="E3" s="2551" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="2411" t="s">
+      <c r="F3" s="2556" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="2416" t="s">
+      <c r="G3" s="2561" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="2421" t="s">
+      <c r="H3" s="2566" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="2426" t="s">
+      <c r="I3" s="2571" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
@@ -12817,25 +13252,25 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="2397" t="s">
+      <c r="C4" s="2542" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2402" t="s">
+      <c r="D4" s="2547" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="2407" t="s">
+      <c r="E4" s="2552" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="2412" t="s">
+      <c r="F4" s="2557" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="2417" t="s">
+      <c r="G4" s="2562" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="2422" t="s">
+      <c r="H4" s="2567" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="2427" t="s">
+      <c r="I4" s="2572" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -12843,25 +13278,25 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="2398" t="s">
+      <c r="C5" s="2543" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2403" t="s">
+      <c r="D5" s="2548" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="2408" t="s">
+      <c r="E5" s="2553" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="2413" t="s">
+      <c r="F5" s="2558" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="2418" t="s">
+      <c r="G5" s="2563" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="2423" t="s">
+      <c r="H5" s="2568" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="2428" t="s">
+      <c r="I5" s="2573" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
@@ -12869,25 +13304,25 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="2399" t="s">
+      <c r="C6" s="2544" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2404" t="s">
+      <c r="D6" s="2549" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="2409" t="s">
+      <c r="E6" s="2554" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="2414" t="s">
+      <c r="F6" s="2559" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="2419" t="s">
+      <c r="G6" s="2564" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="2424" t="s">
+      <c r="H6" s="2569" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="2429" t="s">
+      <c r="I6" s="2574" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
@@ -12895,25 +13330,25 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="2400" t="s">
+      <c r="C7" s="2545" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2405" t="s">
+      <c r="D7" s="2550" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="2410" t="s">
+      <c r="E7" s="2555" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="2415" t="s">
+      <c r="F7" s="2560" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="2420" t="s">
+      <c r="G7" s="2565" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="2425" t="s">
+      <c r="H7" s="2570" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="2430" t="s">
+      <c r="I7" s="2575" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
@@ -14439,31 +14874,31 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="2431" t="s">
+      <c r="C3" s="2576" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2442" t="s">
+      <c r="D3" s="2587" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="2453" t="s">
+      <c r="E3" s="2598" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="2463" t="s">
+      <c r="F3" s="2608" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="2474" t="s">
+      <c r="G3" s="2619" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="2485" t="s">
+      <c r="H3" s="2630" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="2496" t="s">
+      <c r="I3" s="2641" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="2507" t="s">
+      <c r="J3" s="2652" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="2518" t="s">
+      <c r="K3" s="2663" t="s">
         <v>78</v>
       </c>
       <c r="U3" s="8"/>
@@ -14477,31 +14912,31 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="2432" t="s">
+      <c r="C4" s="2577" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2443" t="s">
+      <c r="D4" s="2588" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="2454" t="s">
+      <c r="E4" s="2599" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="2464" t="s">
+      <c r="F4" s="2609" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="2475" t="s">
+      <c r="G4" s="2620" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="2486" t="s">
+      <c r="H4" s="2631" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="2497" t="s">
+      <c r="I4" s="2642" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="2508" t="s">
+      <c r="J4" s="2653" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="2519" t="s">
+      <c r="K4" s="2664" t="s">
         <v>84</v>
       </c>
       <c r="U4" s="8"/>
@@ -14515,31 +14950,31 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="2433" t="s">
+      <c r="C5" s="2578" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2444" t="s">
+      <c r="D5" s="2589" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="2455" t="s">
+      <c r="E5" s="2600" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="2465" t="s">
+      <c r="F5" s="2610" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="2476" t="s">
+      <c r="G5" s="2621" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="2487" t="s">
+      <c r="H5" s="2632" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="2498" t="s">
+      <c r="I5" s="2643" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="2509" t="s">
+      <c r="J5" s="2654" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="2520" t="s">
+      <c r="K5" s="2665" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="8"/>
@@ -14553,31 +14988,31 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="2434" t="s">
+      <c r="C6" s="2579" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2445" t="s">
+      <c r="D6" s="2590" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="2456" t="s">
+      <c r="E6" s="2601" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="2466" t="s">
+      <c r="F6" s="2611" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="2477" t="s">
+      <c r="G6" s="2622" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="2488" t="s">
+      <c r="H6" s="2633" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="2499" t="s">
+      <c r="I6" s="2644" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="2510" t="s">
+      <c r="J6" s="2655" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="2521" t="s">
+      <c r="K6" s="2666" t="s">
         <v>94</v>
       </c>
       <c r="U6" s="8"/>
@@ -14591,29 +15026,29 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="2435" t="s">
+      <c r="C7" s="2580" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2446" t="s">
+      <c r="D7" s="2591" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="2467" t="s">
+      <c r="F7" s="2612" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="2478" t="s">
+      <c r="G7" s="2623" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="2489" t="s">
+      <c r="H7" s="2634" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="2500" t="s">
+      <c r="I7" s="2645" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="2511" t="s">
+      <c r="J7" s="2656" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="2522" t="s">
+      <c r="K7" s="2667" t="s">
         <v>100</v>
       </c>
       <c r="U7" s="8"/>
@@ -14627,31 +15062,31 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="2436" t="s">
+      <c r="C8" s="2581" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2447" t="s">
+      <c r="D8" s="2592" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="2457" t="s">
+      <c r="E8" s="2602" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="2468" t="s">
+      <c r="F8" s="2613" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="2479" t="s">
+      <c r="G8" s="2624" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="2490" t="s">
+      <c r="H8" s="2635" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="2501" t="s">
+      <c r="I8" s="2646" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="2512" t="s">
+      <c r="J8" s="2657" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="2523" t="s">
+      <c r="K8" s="2668" t="s">
         <v>105</v>
       </c>
       <c r="U8" s="8"/>
@@ -14665,31 +15100,31 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="2437" t="s">
+      <c r="C9" s="2582" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2448" t="s">
+      <c r="D9" s="2593" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="2458" t="s">
+      <c r="E9" s="2603" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="2469" t="s">
+      <c r="F9" s="2614" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="2480" t="s">
+      <c r="G9" s="2625" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="2491" t="s">
+      <c r="H9" s="2636" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="2502" t="s">
+      <c r="I9" s="2647" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="2513" t="s">
+      <c r="J9" s="2658" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="2524" t="s">
+      <c r="K9" s="2669" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -14703,31 +15138,31 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="2438" t="s">
+      <c r="C10" s="2583" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2449" t="s">
+      <c r="D10" s="2594" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="2459" t="s">
+      <c r="E10" s="2604" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="2470" t="s">
+      <c r="F10" s="2615" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2481" t="s">
+      <c r="G10" s="2626" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="2492" t="s">
+      <c r="H10" s="2637" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="2503" t="s">
+      <c r="I10" s="2648" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="2514" t="s">
+      <c r="J10" s="2659" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="2525" t="s">
+      <c r="K10" s="2670" t="s">
         <v>115</v>
       </c>
       <c r="U10" s="8"/>
@@ -14741,31 +15176,31 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="2439" t="s">
+      <c r="C11" s="2584" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2450" t="s">
+      <c r="D11" s="2595" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2460" t="s">
+      <c r="E11" s="2605" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="2471" t="s">
+      <c r="F11" s="2616" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="2482" t="s">
+      <c r="G11" s="2627" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="2493" t="s">
+      <c r="H11" s="2638" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="2504" t="s">
+      <c r="I11" s="2649" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="2515" t="s">
+      <c r="J11" s="2660" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="2526" t="s">
+      <c r="K11" s="2671" t="s">
         <v>120</v>
       </c>
       <c r="U11" s="8"/>
@@ -14779,31 +15214,31 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="2440" t="s">
+      <c r="C12" s="2585" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2451" t="s">
+      <c r="D12" s="2596" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="2461" t="s">
+      <c r="E12" s="2606" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="2472" t="s">
+      <c r="F12" s="2617" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="2483" t="s">
+      <c r="G12" s="2628" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="2494" t="s">
+      <c r="H12" s="2639" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="2505" t="s">
+      <c r="I12" s="2650" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="2516" t="s">
+      <c r="J12" s="2661" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="2527" t="s">
+      <c r="K12" s="2672" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="8"/>
@@ -14817,31 +15252,31 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="2441" t="s">
+      <c r="C13" s="2586" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="2452" t="s">
+      <c r="D13" s="2597" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="2462" t="s">
+      <c r="E13" s="2607" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="2473" t="s">
+      <c r="F13" s="2618" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="2484" t="s">
+      <c r="G13" s="2629" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="2495" t="s">
+      <c r="H13" s="2640" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="2506" t="s">
+      <c r="I13" s="2651" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="2517" t="s">
+      <c r="J13" s="2662" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="2528" t="s">
+      <c r="K13" s="2673" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-06-29 15:32:54]  fix markdown relative link paths
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3772" uniqueCount="202">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -997,7 +997,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3254">
+  <cellXfs count="3399">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1122,6 +1122,441 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -13846,44 +14281,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="3109" t="s">
+      <c r="A3" s="3254" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3111" t="s">
+      <c r="B3" s="3256" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3113" t="s">
+      <c r="C3" s="3258" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3115" t="s">
+      <c r="D3" s="3260" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="3117" t="s">
+      <c r="E3" s="3262" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="2539"/>
-      <c r="G3" t="s" s="3119">
+      <c r="G3" t="s" s="3264">
         <v>179</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3110" t="s">
+      <c r="A4" s="3255" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3112" t="s">
+      <c r="B4" s="3257" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3114" t="s">
+      <c r="C4" s="3259" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3116" t="s">
+      <c r="D4" s="3261" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="3118" t="s">
+      <c r="E4" s="3263" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="2540"/>
-      <c r="G4" t="s" s="3120">
+      <c r="G4" t="s" s="3265">
         <v>180</v>
       </c>
     </row>
@@ -15037,135 +15472,135 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="3121" t="s">
+      <c r="C3" s="3266" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3126" t="s">
+      <c r="D3" s="3271" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="3131" t="s">
-        <v>185</v>
+      <c r="E3" s="3276" t="s">
+        <v>181</v>
       </c>
-      <c r="F3" s="3136" t="s">
+      <c r="F3" s="3281" t="s">
         <v>46</v>
       </c>
       <c r="G3" s="2561"/>
-      <c r="H3" s="3141" t="s">
+      <c r="H3" s="3286" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="3146" t="s">
+      <c r="I3" s="3291" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="3151">
+      <c r="K3" t="s" s="3296">
         <v>186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="3122" t="s">
+      <c r="C4" s="3267" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3127" t="s">
+      <c r="D4" s="3272" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="3132" t="s">
-        <v>184</v>
+      <c r="E4" s="3277" t="s">
+        <v>182</v>
       </c>
-      <c r="F4" s="3137" t="s">
+      <c r="F4" s="3282" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="2562"/>
-      <c r="H4" s="3142" t="s">
+      <c r="H4" s="3287" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="3147" t="s">
+      <c r="I4" s="3292" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="3152">
+      <c r="K4" t="s" s="3297">
         <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="3123" t="s">
+      <c r="C5" s="3268" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3128" t="s">
+      <c r="D5" s="3273" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="3133" t="s">
+      <c r="E5" s="3278" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="3138" t="s">
+      <c r="F5" s="3283" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="2563"/>
-      <c r="H5" s="3143" t="s">
+      <c r="H5" s="3288" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="3148" t="s">
+      <c r="I5" s="3293" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
-      <c r="K5" t="s" s="3153">
+      <c r="K5" t="s" s="3298">
         <v>188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="3124" t="s">
+      <c r="C6" s="3269" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3129" t="s">
+      <c r="D6" s="3274" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="3134" t="s">
-        <v>182</v>
+      <c r="E6" s="3279" t="s">
+        <v>184</v>
       </c>
-      <c r="F6" s="3139" t="s">
+      <c r="F6" s="3284" t="s">
         <v>61</v>
       </c>
       <c r="G6" s="2564"/>
-      <c r="H6" s="3144" t="s">
+      <c r="H6" s="3289" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="3149" t="s">
+      <c r="I6" s="3294" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
-      <c r="K6" t="s" s="3154">
+      <c r="K6" t="s" s="3299">
         <v>189</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="3125" t="s">
+      <c r="C7" s="3270" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3130" t="s">
+      <c r="D7" s="3275" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="3135" t="s">
-        <v>181</v>
+      <c r="E7" s="3280" t="s">
+        <v>185</v>
       </c>
-      <c r="F7" s="3140" t="s">
+      <c r="F7" s="3285" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="2565"/>
-      <c r="H7" s="3145" t="s">
+      <c r="H7" s="3290" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="3150" t="s">
+      <c r="I7" s="3295" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
-      <c r="K7" t="s" s="3155">
+      <c r="K7" t="s" s="3300">
         <v>190</v>
       </c>
     </row>
@@ -16690,32 +17125,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="3156" t="s">
+      <c r="C3" s="3301" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3167" t="s">
+      <c r="D3" s="3312" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="3178" t="s">
+      <c r="E3" s="3323" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="3188" t="s">
-        <v>80</v>
+      <c r="F3" s="3333" t="s">
+        <v>95</v>
       </c>
-      <c r="G3" s="3199" t="s">
-        <v>81</v>
+      <c r="G3" s="3344" t="s">
+        <v>96</v>
       </c>
-      <c r="H3" s="3210" t="s">
+      <c r="H3" s="3355" t="s">
         <v>76</v>
       </c>
       <c r="I3" s="2641"/>
-      <c r="J3" s="3221" t="s">
+      <c r="J3" s="3366" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="3232" t="s">
+      <c r="K3" s="3377" t="s">
         <v>78</v>
       </c>
-      <c r="L3" t="s" s="3243">
+      <c r="L3" t="s" s="3388">
         <v>191</v>
       </c>
       <c r="U3" s="8"/>
@@ -16729,32 +17164,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="3157" t="s">
+      <c r="C4" s="3302" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3168" t="s">
+      <c r="D4" s="3313" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="3179" t="s">
+      <c r="E4" s="3324" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="3189" t="s">
-        <v>106</v>
+      <c r="F4" s="3334" t="s">
+        <v>121</v>
       </c>
-      <c r="G4" s="3200" t="s">
-        <v>107</v>
+      <c r="G4" s="3345" t="s">
+        <v>122</v>
       </c>
-      <c r="H4" s="3211" t="s">
+      <c r="H4" s="3356" t="s">
         <v>82</v>
       </c>
       <c r="I4" s="2642"/>
-      <c r="J4" s="3222" t="s">
+      <c r="J4" s="3367" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="3233" t="s">
+      <c r="K4" s="3378" t="s">
         <v>84</v>
       </c>
-      <c r="L4" t="s" s="3244">
+      <c r="L4" t="s" s="3389">
         <v>192</v>
       </c>
       <c r="U4" s="8"/>
@@ -16768,32 +17203,32 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="3158" t="s">
+      <c r="C5" s="3303" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3169" t="s">
+      <c r="D5" s="3314" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="3180" t="s">
+      <c r="E5" s="3325" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="3190" t="s">
-        <v>85</v>
+      <c r="F5" s="3335" t="s">
+        <v>90</v>
       </c>
-      <c r="G5" s="3201" t="s">
-        <v>86</v>
+      <c r="G5" s="3346" t="s">
+        <v>91</v>
       </c>
-      <c r="H5" s="3212" t="s">
+      <c r="H5" s="3357" t="s">
         <v>87</v>
       </c>
       <c r="I5" s="2643"/>
-      <c r="J5" s="3223" t="s">
+      <c r="J5" s="3368" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="3234" t="s">
+      <c r="K5" s="3379" t="s">
         <v>89</v>
       </c>
-      <c r="L5" t="s" s="3245">
+      <c r="L5" t="s" s="3390">
         <v>193</v>
       </c>
       <c r="U5" s="8"/>
@@ -16807,32 +17242,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="3159" t="s">
+      <c r="C6" s="3304" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3170" t="s">
+      <c r="D6" s="3315" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="3181" t="s">
+      <c r="E6" s="3326" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="3191" t="s">
-        <v>90</v>
+      <c r="F6" s="3336" t="s">
+        <v>85</v>
       </c>
-      <c r="G6" s="3202" t="s">
-        <v>91</v>
+      <c r="G6" s="3347" t="s">
+        <v>86</v>
       </c>
-      <c r="H6" s="3213" t="s">
+      <c r="H6" s="3358" t="s">
         <v>92</v>
       </c>
       <c r="I6" s="2644"/>
-      <c r="J6" s="3224" t="s">
+      <c r="J6" s="3369" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="3235" t="s">
+      <c r="K6" s="3380" t="s">
         <v>94</v>
       </c>
-      <c r="L6" t="s" s="3246">
+      <c r="L6" t="s" s="3391">
         <v>194</v>
       </c>
       <c r="U6" s="8"/>
@@ -16846,30 +17281,30 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="3160" t="s">
+      <c r="C7" s="3305" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3171" t="s">
+      <c r="D7" s="3316" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="3192" t="s">
-        <v>121</v>
+      <c r="F7" s="3337" t="s">
+        <v>80</v>
       </c>
-      <c r="G7" s="3203" t="s">
-        <v>122</v>
+      <c r="G7" s="3348" t="s">
+        <v>81</v>
       </c>
-      <c r="H7" s="3214" t="s">
+      <c r="H7" s="3359" t="s">
         <v>97</v>
       </c>
       <c r="I7" s="2645"/>
-      <c r="J7" s="3225" t="s">
+      <c r="J7" s="3370" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="3236" t="s">
+      <c r="K7" s="3381" t="s">
         <v>100</v>
       </c>
-      <c r="L7" t="s" s="3247">
+      <c r="L7" t="s" s="3392">
         <v>195</v>
       </c>
       <c r="U7" s="8"/>
@@ -16883,32 +17318,32 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="3161" t="s">
+      <c r="C8" s="3306" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3172" t="s">
+      <c r="D8" s="3317" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="3182" t="s">
+      <c r="E8" s="3327" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="3193" t="s">
-        <v>126</v>
+      <c r="F8" s="3338" t="s">
+        <v>116</v>
       </c>
-      <c r="G8" s="3204" t="s">
-        <v>127</v>
+      <c r="G8" s="3349" t="s">
+        <v>117</v>
       </c>
-      <c r="H8" s="3215" t="s">
+      <c r="H8" s="3360" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="2646"/>
-      <c r="J8" s="3226" t="s">
+      <c r="J8" s="3371" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="3237" t="s">
+      <c r="K8" s="3382" t="s">
         <v>105</v>
       </c>
-      <c r="L8" t="s" s="3248">
+      <c r="L8" t="s" s="3393">
         <v>196</v>
       </c>
       <c r="U8" s="8"/>
@@ -16922,32 +17357,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="3162" t="s">
+      <c r="C9" s="3307" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="3173" t="s">
+      <c r="D9" s="3318" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="3183" t="s">
+      <c r="E9" s="3328" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="3194" t="s">
-        <v>74</v>
+      <c r="F9" s="3339" t="s">
+        <v>111</v>
       </c>
-      <c r="G9" s="3205" t="s">
-        <v>75</v>
+      <c r="G9" s="3350" t="s">
+        <v>112</v>
       </c>
-      <c r="H9" s="3216" t="s">
+      <c r="H9" s="3361" t="s">
         <v>108</v>
       </c>
       <c r="I9" s="2647"/>
-      <c r="J9" s="3227" t="s">
+      <c r="J9" s="3372" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="3238" t="s">
+      <c r="K9" s="3383" t="s">
         <v>110</v>
       </c>
-      <c r="L9" t="s" s="3249">
+      <c r="L9" t="s" s="3394">
         <v>197</v>
       </c>
       <c r="U9" s="8"/>
@@ -16961,32 +17396,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="3163" t="s">
+      <c r="C10" s="3308" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="3174" t="s">
+      <c r="D10" s="3319" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="3184" t="s">
+      <c r="E10" s="3329" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="3195" t="s">
-        <v>95</v>
+      <c r="F10" s="3340" t="s">
+        <v>74</v>
       </c>
-      <c r="G10" s="3206" t="s">
-        <v>96</v>
+      <c r="G10" s="3351" t="s">
+        <v>75</v>
       </c>
-      <c r="H10" s="3217" t="s">
+      <c r="H10" s="3362" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="2648"/>
-      <c r="J10" s="3228" t="s">
+      <c r="J10" s="3373" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="3239" t="s">
+      <c r="K10" s="3384" t="s">
         <v>115</v>
       </c>
-      <c r="L10" t="s" s="3250">
+      <c r="L10" t="s" s="3395">
         <v>198</v>
       </c>
       <c r="U10" s="8"/>
@@ -17000,32 +17435,32 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="3164" t="s">
+      <c r="C11" s="3309" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="3175" t="s">
+      <c r="D11" s="3320" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="3185" t="s">
+      <c r="E11" s="3330" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="3196" t="s">
-        <v>101</v>
+      <c r="F11" s="3341" t="s">
+        <v>126</v>
       </c>
-      <c r="G11" s="3207" t="s">
-        <v>102</v>
+      <c r="G11" s="3352" t="s">
+        <v>127</v>
       </c>
-      <c r="H11" s="3218" t="s">
+      <c r="H11" s="3363" t="s">
         <v>118</v>
       </c>
       <c r="I11" s="2649"/>
-      <c r="J11" s="3229" t="s">
+      <c r="J11" s="3374" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="3240" t="s">
+      <c r="K11" s="3385" t="s">
         <v>120</v>
       </c>
-      <c r="L11" t="s" s="3251">
+      <c r="L11" t="s" s="3396">
         <v>199</v>
       </c>
       <c r="U11" s="8"/>
@@ -17039,32 +17474,32 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="3165" t="s">
+      <c r="C12" s="3310" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="3176" t="s">
+      <c r="D12" s="3321" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="3186" t="s">
+      <c r="E12" s="3331" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="3197" t="s">
-        <v>111</v>
+      <c r="F12" s="3342" t="s">
+        <v>106</v>
       </c>
-      <c r="G12" s="3208" t="s">
-        <v>112</v>
+      <c r="G12" s="3353" t="s">
+        <v>107</v>
       </c>
-      <c r="H12" s="3219" t="s">
+      <c r="H12" s="3364" t="s">
         <v>123</v>
       </c>
       <c r="I12" s="2650"/>
-      <c r="J12" s="3230" t="s">
+      <c r="J12" s="3375" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="3241" t="s">
+      <c r="K12" s="3386" t="s">
         <v>125</v>
       </c>
-      <c r="L12" t="s" s="3252">
+      <c r="L12" t="s" s="3397">
         <v>200</v>
       </c>
       <c r="U12" s="8"/>
@@ -17078,32 +17513,32 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="3166" t="s">
+      <c r="C13" s="3311" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="3177" t="s">
+      <c r="D13" s="3322" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="3187" t="s">
+      <c r="E13" s="3332" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="3198" t="s">
-        <v>116</v>
+      <c r="F13" s="3343" t="s">
+        <v>101</v>
       </c>
-      <c r="G13" s="3209" t="s">
-        <v>117</v>
+      <c r="G13" s="3354" t="s">
+        <v>102</v>
       </c>
-      <c r="H13" s="3220" t="s">
+      <c r="H13" s="3365" t="s">
         <v>128</v>
       </c>
       <c r="I13" s="2651"/>
-      <c r="J13" s="3231" t="s">
+      <c r="J13" s="3376" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="3242" t="s">
+      <c r="K13" s="3387" t="s">
         <v>130</v>
       </c>
-      <c r="L13" t="s" s="3253">
+      <c r="L13" t="s" s="3398">
         <v>201</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-06-30 11:50:05]  update QuickPrep for all lessons
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3772" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4932" uniqueCount="202">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -997,7 +997,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3399">
+  <cellXfs count="4559">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1122,6 +1122,3486 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -14281,44 +17761,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="3254" t="s">
+      <c r="A3" s="4414" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3256" t="s">
+      <c r="B3" s="4416" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3258" t="s">
+      <c r="C3" s="4418" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3260" t="s">
+      <c r="D3" s="4420" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="3262" t="s">
+      <c r="E3" s="4422" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="2539"/>
-      <c r="G3" t="s" s="3264">
+      <c r="G3" t="s" s="4424">
         <v>179</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3255" t="s">
+      <c r="A4" s="4415" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3257" t="s">
+      <c r="B4" s="4417" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3259" t="s">
+      <c r="C4" s="4419" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3261" t="s">
+      <c r="D4" s="4421" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="3263" t="s">
+      <c r="E4" s="4423" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="2540"/>
-      <c r="G4" t="s" s="3265">
+      <c r="G4" t="s" s="4425">
         <v>180</v>
       </c>
     </row>
@@ -15472,135 +18952,135 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="3266" t="s">
+      <c r="C3" s="4426" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3271" t="s">
+      <c r="D3" s="4431" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="3276" t="s">
+      <c r="E3" s="4436" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="3281" t="s">
+      <c r="F3" s="4441" t="s">
         <v>46</v>
       </c>
       <c r="G3" s="2561"/>
-      <c r="H3" s="3286" t="s">
+      <c r="H3" s="4446" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="3291" t="s">
+      <c r="I3" s="4451" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="3296">
+      <c r="K3" t="s" s="4456">
         <v>186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="3267" t="s">
+      <c r="C4" s="4427" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3272" t="s">
+      <c r="D4" s="4432" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="3277" t="s">
+      <c r="E4" s="4437" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="3282" t="s">
+      <c r="F4" s="4442" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="2562"/>
-      <c r="H4" s="3287" t="s">
+      <c r="H4" s="4447" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="3292" t="s">
+      <c r="I4" s="4452" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="3297">
+      <c r="K4" t="s" s="4457">
         <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="3268" t="s">
+      <c r="C5" s="4428" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3273" t="s">
+      <c r="D5" s="4433" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="3278" t="s">
+      <c r="E5" s="4438" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="3283" t="s">
+      <c r="F5" s="4443" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="2563"/>
-      <c r="H5" s="3288" t="s">
+      <c r="H5" s="4448" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="3293" t="s">
+      <c r="I5" s="4453" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
-      <c r="K5" t="s" s="3298">
+      <c r="K5" t="s" s="4458">
         <v>188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="3269" t="s">
+      <c r="C6" s="4429" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3274" t="s">
+      <c r="D6" s="4434" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="3279" t="s">
+      <c r="E6" s="4439" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="3284" t="s">
+      <c r="F6" s="4444" t="s">
         <v>61</v>
       </c>
       <c r="G6" s="2564"/>
-      <c r="H6" s="3289" t="s">
+      <c r="H6" s="4449" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="3294" t="s">
+      <c r="I6" s="4454" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
-      <c r="K6" t="s" s="3299">
+      <c r="K6" t="s" s="4459">
         <v>189</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="3270" t="s">
+      <c r="C7" s="4430" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3275" t="s">
+      <c r="D7" s="4435" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="3280" t="s">
+      <c r="E7" s="4440" t="s">
         <v>185</v>
       </c>
-      <c r="F7" s="3285" t="s">
+      <c r="F7" s="4445" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="2565"/>
-      <c r="H7" s="3290" t="s">
+      <c r="H7" s="4450" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="3295" t="s">
+      <c r="I7" s="4455" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
-      <c r="K7" t="s" s="3300">
+      <c r="K7" t="s" s="4460">
         <v>190</v>
       </c>
     </row>
@@ -17125,32 +20605,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="3301" t="s">
+      <c r="C3" s="4461" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3312" t="s">
+      <c r="D3" s="4472" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="3323" t="s">
+      <c r="E3" s="4483" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="3333" t="s">
-        <v>95</v>
+      <c r="F3" s="4493" t="s">
+        <v>111</v>
       </c>
-      <c r="G3" s="3344" t="s">
-        <v>96</v>
+      <c r="G3" s="4504" t="s">
+        <v>112</v>
       </c>
-      <c r="H3" s="3355" t="s">
+      <c r="H3" s="4515" t="s">
         <v>76</v>
       </c>
       <c r="I3" s="2641"/>
-      <c r="J3" s="3366" t="s">
+      <c r="J3" s="4526" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="3377" t="s">
+      <c r="K3" s="4537" t="s">
         <v>78</v>
       </c>
-      <c r="L3" t="s" s="3388">
+      <c r="L3" t="s" s="4548">
         <v>191</v>
       </c>
       <c r="U3" s="8"/>
@@ -17164,32 +20644,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="3302" t="s">
+      <c r="C4" s="4462" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3313" t="s">
+      <c r="D4" s="4473" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="3324" t="s">
+      <c r="E4" s="4484" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="3334" t="s">
-        <v>121</v>
+      <c r="F4" s="4494" t="s">
+        <v>95</v>
       </c>
-      <c r="G4" s="3345" t="s">
-        <v>122</v>
+      <c r="G4" s="4505" t="s">
+        <v>96</v>
       </c>
-      <c r="H4" s="3356" t="s">
+      <c r="H4" s="4516" t="s">
         <v>82</v>
       </c>
       <c r="I4" s="2642"/>
-      <c r="J4" s="3367" t="s">
+      <c r="J4" s="4527" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="3378" t="s">
+      <c r="K4" s="4538" t="s">
         <v>84</v>
       </c>
-      <c r="L4" t="s" s="3389">
+      <c r="L4" t="s" s="4549">
         <v>192</v>
       </c>
       <c r="U4" s="8"/>
@@ -17203,32 +20683,32 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="3303" t="s">
+      <c r="C5" s="4463" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3314" t="s">
+      <c r="D5" s="4474" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="3325" t="s">
+      <c r="E5" s="4485" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="3335" t="s">
+      <c r="F5" s="4495" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="3346" t="s">
+      <c r="G5" s="4506" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="3357" t="s">
+      <c r="H5" s="4517" t="s">
         <v>87</v>
       </c>
       <c r="I5" s="2643"/>
-      <c r="J5" s="3368" t="s">
+      <c r="J5" s="4528" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="3379" t="s">
+      <c r="K5" s="4539" t="s">
         <v>89</v>
       </c>
-      <c r="L5" t="s" s="3390">
+      <c r="L5" t="s" s="4550">
         <v>193</v>
       </c>
       <c r="U5" s="8"/>
@@ -17242,32 +20722,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="3304" t="s">
+      <c r="C6" s="4464" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3315" t="s">
+      <c r="D6" s="4475" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="3326" t="s">
+      <c r="E6" s="4486" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="3336" t="s">
+      <c r="F6" s="4496" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="3347" t="s">
+      <c r="G6" s="4507" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="3358" t="s">
+      <c r="H6" s="4518" t="s">
         <v>92</v>
       </c>
       <c r="I6" s="2644"/>
-      <c r="J6" s="3369" t="s">
+      <c r="J6" s="4529" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="3380" t="s">
+      <c r="K6" s="4540" t="s">
         <v>94</v>
       </c>
-      <c r="L6" t="s" s="3391">
+      <c r="L6" t="s" s="4551">
         <v>194</v>
       </c>
       <c r="U6" s="8"/>
@@ -17281,30 +20761,30 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="3305" t="s">
+      <c r="C7" s="4465" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3316" t="s">
+      <c r="D7" s="4476" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="3337" t="s">
-        <v>80</v>
+      <c r="F7" s="4497" t="s">
+        <v>74</v>
       </c>
-      <c r="G7" s="3348" t="s">
-        <v>81</v>
+      <c r="G7" s="4508" t="s">
+        <v>75</v>
       </c>
-      <c r="H7" s="3359" t="s">
+      <c r="H7" s="4519" t="s">
         <v>97</v>
       </c>
       <c r="I7" s="2645"/>
-      <c r="J7" s="3370" t="s">
+      <c r="J7" s="4530" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="3381" t="s">
+      <c r="K7" s="4541" t="s">
         <v>100</v>
       </c>
-      <c r="L7" t="s" s="3392">
+      <c r="L7" t="s" s="4552">
         <v>195</v>
       </c>
       <c r="U7" s="8"/>
@@ -17318,32 +20798,32 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="3306" t="s">
+      <c r="C8" s="4466" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3317" t="s">
+      <c r="D8" s="4477" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="3327" t="s">
+      <c r="E8" s="4487" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="3338" t="s">
-        <v>116</v>
+      <c r="F8" s="4498" t="s">
+        <v>126</v>
       </c>
-      <c r="G8" s="3349" t="s">
-        <v>117</v>
+      <c r="G8" s="4509" t="s">
+        <v>127</v>
       </c>
-      <c r="H8" s="3360" t="s">
+      <c r="H8" s="4520" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="2646"/>
-      <c r="J8" s="3371" t="s">
+      <c r="J8" s="4531" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="3382" t="s">
+      <c r="K8" s="4542" t="s">
         <v>105</v>
       </c>
-      <c r="L8" t="s" s="3393">
+      <c r="L8" t="s" s="4553">
         <v>196</v>
       </c>
       <c r="U8" s="8"/>
@@ -17357,32 +20837,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="3307" t="s">
+      <c r="C9" s="4467" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="3318" t="s">
+      <c r="D9" s="4478" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="3328" t="s">
+      <c r="E9" s="4488" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="3339" t="s">
-        <v>111</v>
+      <c r="F9" s="4499" t="s">
+        <v>121</v>
       </c>
-      <c r="G9" s="3350" t="s">
-        <v>112</v>
+      <c r="G9" s="4510" t="s">
+        <v>122</v>
       </c>
-      <c r="H9" s="3361" t="s">
+      <c r="H9" s="4521" t="s">
         <v>108</v>
       </c>
       <c r="I9" s="2647"/>
-      <c r="J9" s="3372" t="s">
+      <c r="J9" s="4532" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="3383" t="s">
+      <c r="K9" s="4543" t="s">
         <v>110</v>
       </c>
-      <c r="L9" t="s" s="3394">
+      <c r="L9" t="s" s="4554">
         <v>197</v>
       </c>
       <c r="U9" s="8"/>
@@ -17396,32 +20876,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="3308" t="s">
+      <c r="C10" s="4468" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="3319" t="s">
+      <c r="D10" s="4479" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="3329" t="s">
+      <c r="E10" s="4489" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="3340" t="s">
-        <v>74</v>
+      <c r="F10" s="4500" t="s">
+        <v>106</v>
       </c>
-      <c r="G10" s="3351" t="s">
-        <v>75</v>
+      <c r="G10" s="4511" t="s">
+        <v>107</v>
       </c>
-      <c r="H10" s="3362" t="s">
+      <c r="H10" s="4522" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="2648"/>
-      <c r="J10" s="3373" t="s">
+      <c r="J10" s="4533" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="3384" t="s">
+      <c r="K10" s="4544" t="s">
         <v>115</v>
       </c>
-      <c r="L10" t="s" s="3395">
+      <c r="L10" t="s" s="4555">
         <v>198</v>
       </c>
       <c r="U10" s="8"/>
@@ -17435,32 +20915,32 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="3309" t="s">
+      <c r="C11" s="4469" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="3320" t="s">
+      <c r="D11" s="4480" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="3330" t="s">
+      <c r="E11" s="4490" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="3341" t="s">
-        <v>126</v>
+      <c r="F11" s="4501" t="s">
+        <v>101</v>
       </c>
-      <c r="G11" s="3352" t="s">
-        <v>127</v>
+      <c r="G11" s="4512" t="s">
+        <v>102</v>
       </c>
-      <c r="H11" s="3363" t="s">
+      <c r="H11" s="4523" t="s">
         <v>118</v>
       </c>
       <c r="I11" s="2649"/>
-      <c r="J11" s="3374" t="s">
+      <c r="J11" s="4534" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="3385" t="s">
+      <c r="K11" s="4545" t="s">
         <v>120</v>
       </c>
-      <c r="L11" t="s" s="3396">
+      <c r="L11" t="s" s="4556">
         <v>199</v>
       </c>
       <c r="U11" s="8"/>
@@ -17474,32 +20954,32 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="3310" t="s">
+      <c r="C12" s="4470" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="3321" t="s">
+      <c r="D12" s="4481" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="3331" t="s">
+      <c r="E12" s="4491" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="3342" t="s">
-        <v>106</v>
+      <c r="F12" s="4502" t="s">
+        <v>80</v>
       </c>
-      <c r="G12" s="3353" t="s">
-        <v>107</v>
+      <c r="G12" s="4513" t="s">
+        <v>81</v>
       </c>
-      <c r="H12" s="3364" t="s">
+      <c r="H12" s="4524" t="s">
         <v>123</v>
       </c>
       <c r="I12" s="2650"/>
-      <c r="J12" s="3375" t="s">
+      <c r="J12" s="4535" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="3386" t="s">
+      <c r="K12" s="4546" t="s">
         <v>125</v>
       </c>
-      <c r="L12" t="s" s="3397">
+      <c r="L12" t="s" s="4557">
         <v>200</v>
       </c>
       <c r="U12" s="8"/>
@@ -17513,32 +20993,32 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="3311" t="s">
+      <c r="C13" s="4471" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="3322" t="s">
+      <c r="D13" s="4482" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="3332" t="s">
+      <c r="E13" s="4492" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="3343" t="s">
-        <v>101</v>
+      <c r="F13" s="4503" t="s">
+        <v>116</v>
       </c>
-      <c r="G13" s="3354" t="s">
-        <v>102</v>
+      <c r="G13" s="4514" t="s">
+        <v>117</v>
       </c>
-      <c r="H13" s="3365" t="s">
+      <c r="H13" s="4525" t="s">
         <v>128</v>
       </c>
       <c r="I13" s="2651"/>
-      <c r="J13" s="3376" t="s">
+      <c r="J13" s="4536" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="3387" t="s">
+      <c r="K13" s="4547" t="s">
         <v>130</v>
       </c>
-      <c r="L13" t="s" s="3398">
+      <c r="L13" t="s" s="4558">
         <v>201</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-07-15 23:24:05]  All projects rebuilt with DefaultLocale
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5077" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5512" uniqueCount="202">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -997,7 +997,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4704">
+  <cellXfs count="5139">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1122,6 +1122,1311 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -18196,44 +19501,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="4559" t="s">
+      <c r="A3" s="4994" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4561" t="s">
+      <c r="B3" s="4996" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="4563" t="s">
+      <c r="C3" s="4998" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4565" t="s">
+      <c r="D3" s="5000" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="4567" t="s">
+      <c r="E3" s="5002" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="2539"/>
-      <c r="G3" t="s" s="4569">
+      <c r="G3" t="s" s="5004">
         <v>179</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4560" t="s">
+      <c r="A4" s="4995" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4562" t="s">
+      <c r="B4" s="4997" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="4564" t="s">
+      <c r="C4" s="4999" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4566" t="s">
+      <c r="D4" s="5001" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="4568" t="s">
+      <c r="E4" s="5003" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="2540"/>
-      <c r="G4" t="s" s="4570">
+      <c r="G4" t="s" s="5005">
         <v>180</v>
       </c>
     </row>
@@ -19387,135 +20692,135 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="4571" t="s">
+      <c r="C3" s="5006" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="4576" t="s">
+      <c r="D3" s="5011" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="4581" t="s">
-        <v>185</v>
+      <c r="E3" s="5016" t="s">
+        <v>181</v>
       </c>
-      <c r="F3" s="4586" t="s">
+      <c r="F3" s="5021" t="s">
         <v>46</v>
       </c>
       <c r="G3" s="2561"/>
-      <c r="H3" s="4591" t="s">
+      <c r="H3" s="5026" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="4596" t="s">
+      <c r="I3" s="5031" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="4601">
+      <c r="K3" t="s" s="5036">
         <v>186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="4572" t="s">
+      <c r="C4" s="5007" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="4577" t="s">
+      <c r="D4" s="5012" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="4582" t="s">
-        <v>184</v>
+      <c r="E4" s="5017" t="s">
+        <v>182</v>
       </c>
-      <c r="F4" s="4587" t="s">
+      <c r="F4" s="5022" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="2562"/>
-      <c r="H4" s="4592" t="s">
+      <c r="H4" s="5027" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="4597" t="s">
+      <c r="I4" s="5032" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="4602">
+      <c r="K4" t="s" s="5037">
         <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="4573" t="s">
+      <c r="C5" s="5008" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="4578" t="s">
+      <c r="D5" s="5013" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="4583" t="s">
+      <c r="E5" s="5018" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="4588" t="s">
+      <c r="F5" s="5023" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="2563"/>
-      <c r="H5" s="4593" t="s">
+      <c r="H5" s="5028" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="4598" t="s">
+      <c r="I5" s="5033" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
-      <c r="K5" t="s" s="4603">
+      <c r="K5" t="s" s="5038">
         <v>188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="4574" t="s">
+      <c r="C6" s="5009" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="4579" t="s">
+      <c r="D6" s="5014" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="4584" t="s">
-        <v>182</v>
+      <c r="E6" s="5019" t="s">
+        <v>184</v>
       </c>
-      <c r="F6" s="4589" t="s">
+      <c r="F6" s="5024" t="s">
         <v>61</v>
       </c>
       <c r="G6" s="2564"/>
-      <c r="H6" s="4594" t="s">
+      <c r="H6" s="5029" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="4599" t="s">
+      <c r="I6" s="5034" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
-      <c r="K6" t="s" s="4604">
+      <c r="K6" t="s" s="5039">
         <v>189</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="4575" t="s">
+      <c r="C7" s="5010" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="4580" t="s">
+      <c r="D7" s="5015" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="4585" t="s">
-        <v>181</v>
+      <c r="E7" s="5020" t="s">
+        <v>185</v>
       </c>
-      <c r="F7" s="4590" t="s">
+      <c r="F7" s="5025" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="2565"/>
-      <c r="H7" s="4595" t="s">
+      <c r="H7" s="5030" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="4600" t="s">
+      <c r="I7" s="5035" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
-      <c r="K7" t="s" s="4605">
+      <c r="K7" t="s" s="5040">
         <v>190</v>
       </c>
     </row>
@@ -21040,32 +22345,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="4606" t="s">
+      <c r="C3" s="5041" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="4617" t="s">
+      <c r="D3" s="5052" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="4628" t="s">
+      <c r="E3" s="5063" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="4638" t="s">
-        <v>106</v>
+      <c r="F3" s="5073" t="s">
+        <v>95</v>
       </c>
-      <c r="G3" s="4649" t="s">
-        <v>107</v>
+      <c r="G3" s="5084" t="s">
+        <v>96</v>
       </c>
-      <c r="H3" s="4660" t="s">
+      <c r="H3" s="5095" t="s">
         <v>76</v>
       </c>
       <c r="I3" s="2641"/>
-      <c r="J3" s="4671" t="s">
+      <c r="J3" s="5106" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="4682" t="s">
+      <c r="K3" s="5117" t="s">
         <v>78</v>
       </c>
-      <c r="L3" t="s" s="4693">
+      <c r="L3" t="s" s="5128">
         <v>191</v>
       </c>
       <c r="U3" s="8"/>
@@ -21079,32 +22384,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="4607" t="s">
+      <c r="C4" s="5042" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="4618" t="s">
+      <c r="D4" s="5053" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="4629" t="s">
+      <c r="E4" s="5064" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="4639" t="s">
-        <v>74</v>
+      <c r="F4" s="5074" t="s">
+        <v>121</v>
       </c>
-      <c r="G4" s="4650" t="s">
-        <v>75</v>
+      <c r="G4" s="5085" t="s">
+        <v>122</v>
       </c>
-      <c r="H4" s="4661" t="s">
+      <c r="H4" s="5096" t="s">
         <v>82</v>
       </c>
       <c r="I4" s="2642"/>
-      <c r="J4" s="4672" t="s">
+      <c r="J4" s="5107" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="4683" t="s">
+      <c r="K4" s="5118" t="s">
         <v>84</v>
       </c>
-      <c r="L4" t="s" s="4694">
+      <c r="L4" t="s" s="5129">
         <v>192</v>
       </c>
       <c r="U4" s="8"/>
@@ -21118,32 +22423,32 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="4608" t="s">
+      <c r="C5" s="5043" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="4619" t="s">
+      <c r="D5" s="5054" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="4630" t="s">
+      <c r="E5" s="5065" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="4640" t="s">
-        <v>85</v>
+      <c r="F5" s="5075" t="s">
+        <v>90</v>
       </c>
-      <c r="G5" s="4651" t="s">
-        <v>86</v>
+      <c r="G5" s="5086" t="s">
+        <v>91</v>
       </c>
-      <c r="H5" s="4662" t="s">
+      <c r="H5" s="5097" t="s">
         <v>87</v>
       </c>
       <c r="I5" s="2643"/>
-      <c r="J5" s="4673" t="s">
+      <c r="J5" s="5108" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="4684" t="s">
+      <c r="K5" s="5119" t="s">
         <v>89</v>
       </c>
-      <c r="L5" t="s" s="4695">
+      <c r="L5" t="s" s="5130">
         <v>193</v>
       </c>
       <c r="U5" s="8"/>
@@ -21157,32 +22462,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="4609" t="s">
+      <c r="C6" s="5044" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="4620" t="s">
+      <c r="D6" s="5055" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="4631" t="s">
+      <c r="E6" s="5066" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="4641" t="s">
-        <v>90</v>
+      <c r="F6" s="5076" t="s">
+        <v>85</v>
       </c>
-      <c r="G6" s="4652" t="s">
-        <v>91</v>
+      <c r="G6" s="5087" t="s">
+        <v>86</v>
       </c>
-      <c r="H6" s="4663" t="s">
+      <c r="H6" s="5098" t="s">
         <v>92</v>
       </c>
       <c r="I6" s="2644"/>
-      <c r="J6" s="4674" t="s">
+      <c r="J6" s="5109" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="4685" t="s">
+      <c r="K6" s="5120" t="s">
         <v>94</v>
       </c>
-      <c r="L6" t="s" s="4696">
+      <c r="L6" t="s" s="5131">
         <v>194</v>
       </c>
       <c r="U6" s="8"/>
@@ -21196,30 +22501,30 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="4610" t="s">
+      <c r="C7" s="5045" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="4621" t="s">
+      <c r="D7" s="5056" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="4642" t="s">
-        <v>111</v>
+      <c r="F7" s="5077" t="s">
+        <v>80</v>
       </c>
-      <c r="G7" s="4653" t="s">
-        <v>112</v>
+      <c r="G7" s="5088" t="s">
+        <v>81</v>
       </c>
-      <c r="H7" s="4664" t="s">
+      <c r="H7" s="5099" t="s">
         <v>97</v>
       </c>
       <c r="I7" s="2645"/>
-      <c r="J7" s="4675" t="s">
+      <c r="J7" s="5110" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="4686" t="s">
+      <c r="K7" s="5121" t="s">
         <v>100</v>
       </c>
-      <c r="L7" t="s" s="4697">
+      <c r="L7" t="s" s="5132">
         <v>195</v>
       </c>
       <c r="U7" s="8"/>
@@ -21233,32 +22538,32 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="4611" t="s">
+      <c r="C8" s="5046" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="4622" t="s">
+      <c r="D8" s="5057" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="4632" t="s">
+      <c r="E8" s="5067" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="4643" t="s">
+      <c r="F8" s="5078" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="4654" t="s">
+      <c r="G8" s="5089" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="4665" t="s">
+      <c r="H8" s="5100" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="2646"/>
-      <c r="J8" s="4676" t="s">
+      <c r="J8" s="5111" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="4687" t="s">
+      <c r="K8" s="5122" t="s">
         <v>105</v>
       </c>
-      <c r="L8" t="s" s="4698">
+      <c r="L8" t="s" s="5133">
         <v>196</v>
       </c>
       <c r="U8" s="8"/>
@@ -21272,32 +22577,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="4612" t="s">
+      <c r="C9" s="5047" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4623" t="s">
+      <c r="D9" s="5058" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="4633" t="s">
+      <c r="E9" s="5068" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="4644" t="s">
-        <v>80</v>
+      <c r="F9" s="5079" t="s">
+        <v>111</v>
       </c>
-      <c r="G9" s="4655" t="s">
-        <v>81</v>
+      <c r="G9" s="5090" t="s">
+        <v>112</v>
       </c>
-      <c r="H9" s="4666" t="s">
+      <c r="H9" s="5101" t="s">
         <v>108</v>
       </c>
       <c r="I9" s="2647"/>
-      <c r="J9" s="4677" t="s">
+      <c r="J9" s="5112" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="4688" t="s">
+      <c r="K9" s="5123" t="s">
         <v>110</v>
       </c>
-      <c r="L9" t="s" s="4699">
+      <c r="L9" t="s" s="5134">
         <v>197</v>
       </c>
       <c r="U9" s="8"/>
@@ -21311,32 +22616,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="4613" t="s">
+      <c r="C10" s="5048" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="4624" t="s">
+      <c r="D10" s="5059" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="4634" t="s">
+      <c r="E10" s="5069" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="4645" t="s">
-        <v>121</v>
+      <c r="F10" s="5080" t="s">
+        <v>74</v>
       </c>
-      <c r="G10" s="4656" t="s">
-        <v>122</v>
+      <c r="G10" s="5091" t="s">
+        <v>75</v>
       </c>
-      <c r="H10" s="4667" t="s">
+      <c r="H10" s="5102" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="2648"/>
-      <c r="J10" s="4678" t="s">
+      <c r="J10" s="5113" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="4689" t="s">
+      <c r="K10" s="5124" t="s">
         <v>115</v>
       </c>
-      <c r="L10" t="s" s="4700">
+      <c r="L10" t="s" s="5135">
         <v>198</v>
       </c>
       <c r="U10" s="8"/>
@@ -21350,32 +22655,32 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="4614" t="s">
+      <c r="C11" s="5049" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="4625" t="s">
+      <c r="D11" s="5060" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="4635" t="s">
+      <c r="E11" s="5070" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="4646" t="s">
+      <c r="F11" s="5081" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="4657" t="s">
+      <c r="G11" s="5092" t="s">
         <v>127</v>
       </c>
-      <c r="H11" s="4668" t="s">
+      <c r="H11" s="5103" t="s">
         <v>118</v>
       </c>
       <c r="I11" s="2649"/>
-      <c r="J11" s="4679" t="s">
+      <c r="J11" s="5114" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="4690" t="s">
+      <c r="K11" s="5125" t="s">
         <v>120</v>
       </c>
-      <c r="L11" t="s" s="4701">
+      <c r="L11" t="s" s="5136">
         <v>199</v>
       </c>
       <c r="U11" s="8"/>
@@ -21389,32 +22694,32 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="4615" t="s">
+      <c r="C12" s="5050" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4626" t="s">
+      <c r="D12" s="5061" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="4636" t="s">
+      <c r="E12" s="5071" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="4647" t="s">
-        <v>95</v>
+      <c r="F12" s="5082" t="s">
+        <v>106</v>
       </c>
-      <c r="G12" s="4658" t="s">
-        <v>96</v>
+      <c r="G12" s="5093" t="s">
+        <v>107</v>
       </c>
-      <c r="H12" s="4669" t="s">
+      <c r="H12" s="5104" t="s">
         <v>123</v>
       </c>
       <c r="I12" s="2650"/>
-      <c r="J12" s="4680" t="s">
+      <c r="J12" s="5115" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="4691" t="s">
+      <c r="K12" s="5126" t="s">
         <v>125</v>
       </c>
-      <c r="L12" t="s" s="4702">
+      <c r="L12" t="s" s="5137">
         <v>200</v>
       </c>
       <c r="U12" s="8"/>
@@ -21428,32 +22733,32 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="4616" t="s">
+      <c r="C13" s="5051" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4627" t="s">
+      <c r="D13" s="5062" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="4637" t="s">
+      <c r="E13" s="5072" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="4648" t="s">
+      <c r="F13" s="5083" t="s">
         <v>101</v>
       </c>
-      <c r="G13" s="4659" t="s">
+      <c r="G13" s="5094" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="4670" t="s">
+      <c r="H13" s="5105" t="s">
         <v>128</v>
       </c>
       <c r="I13" s="2651"/>
-      <c r="J13" s="4681" t="s">
+      <c r="J13" s="5116" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="4692" t="s">
+      <c r="K13" s="5127" t="s">
         <v>130</v>
       </c>
-      <c r="L13" t="s" s="4703">
+      <c r="L13" t="s" s="5138">
         <v>201</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-07-26 17:58:58] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5512" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5947" uniqueCount="213">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -697,6 +697,39 @@
   <si>
     <t>17pVB3Aty3FHTRtH5-3ntvluGNMv_HBBuuruTBezuoQk</t>
   </si>
+  <si>
+    <t>https://docs.google.com/document/d/1pV0IRpph3dnb8V-o0uKfuNjedNV8BFsdNBoG2BSKK0o/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1QOCEvwIk8366_VK18TnXMCyqDyy9sx6D12q5xjcGK_U/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1522hLLXRKBO8VzALl6WXv4WyuNa_I1jAJormI5tOuH8/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1HkWzEQB69xulxAWz2Xh5tnpDa2Uwj9JSZnLIhJuEMFA/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1rwgBdQ3W9XKdhfEddiBGs5vRxtTDOthOiSZAgNILqUw/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/15hzLjht_9G8jfyDMk6ybpdDbJeYMO9O-wvhoOgx9ly8/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1_3YoCjZOVkdEkiiyiAn7cOxIgezulVlYyWT3ChPMYr8/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1y5be2mif380Ee1XpI3dzyTn2WsrVm4zhe95XcG1XHYg/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1zgylTvNDPslFcPwWyujTkgJphW7GmLrj-QoiirYJ-MA/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1ZAoZ_E2Jm6R5zI9fswxCorDS4AiCi9bxlvAZxrFGysY/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/17pVB3Aty3FHTRtH5-3ntvluGNMv_HBBuuruTBezuoQk/template/preview</t>
+  </si>
 </sst>
 </file>
 
@@ -997,7 +1030,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5139">
+  <cellXfs count="5574">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1122,6 +1155,1311 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -19501,44 +20839,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="4994" t="s">
+      <c r="A3" s="5429" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4996" t="s">
+      <c r="B3" s="5431" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="4998" t="s">
+      <c r="C3" s="5433" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="5000" t="s">
+      <c r="D3" s="5435" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="5002" t="s">
+      <c r="E3" s="5437" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="2539"/>
-      <c r="G3" t="s" s="5004">
+      <c r="G3" t="s" s="5439">
         <v>179</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4995" t="s">
+      <c r="A4" s="5430" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4997" t="s">
+      <c r="B4" s="5432" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="4999" t="s">
+      <c r="C4" s="5434" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="5001" t="s">
+      <c r="D4" s="5436" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="5003" t="s">
+      <c r="E4" s="5438" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="2540"/>
-      <c r="G4" t="s" s="5005">
+      <c r="G4" t="s" s="5440">
         <v>180</v>
       </c>
     </row>
@@ -20692,135 +22030,135 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="5006" t="s">
+      <c r="C3" s="5441" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="5011" t="s">
+      <c r="D3" s="5446" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="5016" t="s">
+      <c r="E3" s="5451" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="5021" t="s">
+      <c r="F3" s="5456" t="s">
         <v>46</v>
       </c>
       <c r="G3" s="2561"/>
-      <c r="H3" s="5026" t="s">
+      <c r="H3" s="5461" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="5031" t="s">
+      <c r="I3" s="5466" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="5036">
+      <c r="K3" t="s" s="5471">
         <v>186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="5007" t="s">
+      <c r="C4" s="5442" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="5012" t="s">
+      <c r="D4" s="5447" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="5017" t="s">
+      <c r="E4" s="5452" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="5022" t="s">
+      <c r="F4" s="5457" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="2562"/>
-      <c r="H4" s="5027" t="s">
+      <c r="H4" s="5462" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="5032" t="s">
+      <c r="I4" s="5467" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="5037">
+      <c r="K4" t="s" s="5472">
         <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="5008" t="s">
+      <c r="C5" s="5443" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="5013" t="s">
+      <c r="D5" s="5448" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="5018" t="s">
+      <c r="E5" s="5453" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="5023" t="s">
+      <c r="F5" s="5458" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="2563"/>
-      <c r="H5" s="5028" t="s">
+      <c r="H5" s="5463" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="5033" t="s">
+      <c r="I5" s="5468" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
-      <c r="K5" t="s" s="5038">
+      <c r="K5" t="s" s="5473">
         <v>188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="5009" t="s">
+      <c r="C6" s="5444" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="5014" t="s">
+      <c r="D6" s="5449" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="5019" t="s">
+      <c r="E6" s="5454" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="5024" t="s">
+      <c r="F6" s="5459" t="s">
         <v>61</v>
       </c>
       <c r="G6" s="2564"/>
-      <c r="H6" s="5029" t="s">
+      <c r="H6" s="5464" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="5034" t="s">
+      <c r="I6" s="5469" t="s">
         <v>63</v>
       </c>
       <c r="J6"/>
-      <c r="K6" t="s" s="5039">
+      <c r="K6" t="s" s="5474">
         <v>189</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="5010" t="s">
+      <c r="C7" s="5445" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="5015" t="s">
+      <c r="D7" s="5450" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="5020" t="s">
+      <c r="E7" s="5455" t="s">
         <v>185</v>
       </c>
-      <c r="F7" s="5025" t="s">
+      <c r="F7" s="5460" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="2565"/>
-      <c r="H7" s="5030" t="s">
+      <c r="H7" s="5465" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="5035" t="s">
+      <c r="I7" s="5470" t="s">
         <v>68</v>
       </c>
       <c r="J7"/>
-      <c r="K7" t="s" s="5040">
+      <c r="K7" t="s" s="5475">
         <v>190</v>
       </c>
     </row>
@@ -22345,32 +23683,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="5041" t="s">
+      <c r="C3" s="5476" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="5052" t="s">
+      <c r="D3" s="5487" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="5063" t="s">
+      <c r="E3" s="5498" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="5073" t="s">
-        <v>95</v>
+      <c r="F3" s="5508" t="s">
+        <v>74</v>
       </c>
-      <c r="G3" s="5084" t="s">
-        <v>96</v>
+      <c r="G3" s="5519" t="s">
+        <v>75</v>
       </c>
-      <c r="H3" s="5095" t="s">
+      <c r="H3" s="5530" t="s">
         <v>76</v>
       </c>
       <c r="I3" s="2641"/>
-      <c r="J3" s="5106" t="s">
-        <v>77</v>
+      <c r="J3" s="5541" t="s">
+        <v>202</v>
       </c>
-      <c r="K3" s="5117" t="s">
+      <c r="K3" s="5552" t="s">
         <v>78</v>
       </c>
-      <c r="L3" t="s" s="5128">
+      <c r="L3" t="s" s="5563">
         <v>191</v>
       </c>
       <c r="U3" s="8"/>
@@ -22384,32 +23722,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="5042" t="s">
+      <c r="C4" s="5477" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="5053" t="s">
+      <c r="D4" s="5488" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="5064" t="s">
+      <c r="E4" s="5499" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="5074" t="s">
-        <v>121</v>
+      <c r="F4" s="5509" t="s">
+        <v>80</v>
       </c>
-      <c r="G4" s="5085" t="s">
-        <v>122</v>
+      <c r="G4" s="5520" t="s">
+        <v>81</v>
       </c>
-      <c r="H4" s="5096" t="s">
+      <c r="H4" s="5531" t="s">
         <v>82</v>
       </c>
       <c r="I4" s="2642"/>
-      <c r="J4" s="5107" t="s">
-        <v>83</v>
+      <c r="J4" s="5542" t="s">
+        <v>203</v>
       </c>
-      <c r="K4" s="5118" t="s">
+      <c r="K4" s="5553" t="s">
         <v>84</v>
       </c>
-      <c r="L4" t="s" s="5129">
+      <c r="L4" t="s" s="5564">
         <v>192</v>
       </c>
       <c r="U4" s="8"/>
@@ -22423,32 +23761,32 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="5043" t="s">
+      <c r="C5" s="5478" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="5054" t="s">
+      <c r="D5" s="5489" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="5065" t="s">
+      <c r="E5" s="5500" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="5075" t="s">
-        <v>90</v>
+      <c r="F5" s="5510" t="s">
+        <v>85</v>
       </c>
-      <c r="G5" s="5086" t="s">
-        <v>91</v>
+      <c r="G5" s="5521" t="s">
+        <v>86</v>
       </c>
-      <c r="H5" s="5097" t="s">
+      <c r="H5" s="5532" t="s">
         <v>87</v>
       </c>
       <c r="I5" s="2643"/>
-      <c r="J5" s="5108" t="s">
-        <v>88</v>
+      <c r="J5" s="5543" t="s">
+        <v>204</v>
       </c>
-      <c r="K5" s="5119" t="s">
+      <c r="K5" s="5554" t="s">
         <v>89</v>
       </c>
-      <c r="L5" t="s" s="5130">
+      <c r="L5" t="s" s="5565">
         <v>193</v>
       </c>
       <c r="U5" s="8"/>
@@ -22462,32 +23800,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="5044" t="s">
+      <c r="C6" s="5479" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="5055" t="s">
+      <c r="D6" s="5490" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="5066" t="s">
+      <c r="E6" s="5501" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="5076" t="s">
-        <v>85</v>
+      <c r="F6" s="5511" t="s">
+        <v>90</v>
       </c>
-      <c r="G6" s="5087" t="s">
-        <v>86</v>
+      <c r="G6" s="5522" t="s">
+        <v>91</v>
       </c>
-      <c r="H6" s="5098" t="s">
+      <c r="H6" s="5533" t="s">
         <v>92</v>
       </c>
       <c r="I6" s="2644"/>
-      <c r="J6" s="5109" t="s">
-        <v>93</v>
+      <c r="J6" s="5544" t="s">
+        <v>205</v>
       </c>
-      <c r="K6" s="5120" t="s">
+      <c r="K6" s="5555" t="s">
         <v>94</v>
       </c>
-      <c r="L6" t="s" s="5131">
+      <c r="L6" t="s" s="5566">
         <v>194</v>
       </c>
       <c r="U6" s="8"/>
@@ -22501,30 +23839,30 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="5045" t="s">
+      <c r="C7" s="5480" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="5056" t="s">
+      <c r="D7" s="5491" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="5077" t="s">
-        <v>80</v>
+      <c r="F7" s="5512" t="s">
+        <v>95</v>
       </c>
-      <c r="G7" s="5088" t="s">
-        <v>81</v>
+      <c r="G7" s="5523" t="s">
+        <v>96</v>
       </c>
-      <c r="H7" s="5099" t="s">
+      <c r="H7" s="5534" t="s">
         <v>97</v>
       </c>
       <c r="I7" s="2645"/>
-      <c r="J7" s="5110" t="s">
-        <v>99</v>
+      <c r="J7" s="5545" t="s">
+        <v>206</v>
       </c>
-      <c r="K7" s="5121" t="s">
+      <c r="K7" s="5556" t="s">
         <v>100</v>
       </c>
-      <c r="L7" t="s" s="5132">
+      <c r="L7" t="s" s="5567">
         <v>195</v>
       </c>
       <c r="U7" s="8"/>
@@ -22538,32 +23876,32 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="5046" t="s">
+      <c r="C8" s="5481" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="5057" t="s">
+      <c r="D8" s="5492" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="5067" t="s">
+      <c r="E8" s="5502" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="5078" t="s">
-        <v>116</v>
+      <c r="F8" s="5513" t="s">
+        <v>101</v>
       </c>
-      <c r="G8" s="5089" t="s">
-        <v>117</v>
+      <c r="G8" s="5524" t="s">
+        <v>102</v>
       </c>
-      <c r="H8" s="5100" t="s">
+      <c r="H8" s="5535" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="2646"/>
-      <c r="J8" s="5111" t="s">
-        <v>104</v>
+      <c r="J8" s="5546" t="s">
+        <v>207</v>
       </c>
-      <c r="K8" s="5122" t="s">
+      <c r="K8" s="5557" t="s">
         <v>105</v>
       </c>
-      <c r="L8" t="s" s="5133">
+      <c r="L8" t="s" s="5568">
         <v>196</v>
       </c>
       <c r="U8" s="8"/>
@@ -22577,32 +23915,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="5047" t="s">
+      <c r="C9" s="5482" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="5058" t="s">
+      <c r="D9" s="5493" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="5068" t="s">
+      <c r="E9" s="5503" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="5079" t="s">
-        <v>111</v>
+      <c r="F9" s="5514" t="s">
+        <v>106</v>
       </c>
-      <c r="G9" s="5090" t="s">
-        <v>112</v>
+      <c r="G9" s="5525" t="s">
+        <v>107</v>
       </c>
-      <c r="H9" s="5101" t="s">
+      <c r="H9" s="5536" t="s">
         <v>108</v>
       </c>
       <c r="I9" s="2647"/>
-      <c r="J9" s="5112" t="s">
-        <v>109</v>
+      <c r="J9" s="5547" t="s">
+        <v>208</v>
       </c>
-      <c r="K9" s="5123" t="s">
+      <c r="K9" s="5558" t="s">
         <v>110</v>
       </c>
-      <c r="L9" t="s" s="5134">
+      <c r="L9" t="s" s="5569">
         <v>197</v>
       </c>
       <c r="U9" s="8"/>
@@ -22616,32 +23954,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="5048" t="s">
+      <c r="C10" s="5483" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="5059" t="s">
+      <c r="D10" s="5494" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="5069" t="s">
+      <c r="E10" s="5504" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="5080" t="s">
-        <v>74</v>
+      <c r="F10" s="5515" t="s">
+        <v>111</v>
       </c>
-      <c r="G10" s="5091" t="s">
-        <v>75</v>
+      <c r="G10" s="5526" t="s">
+        <v>112</v>
       </c>
-      <c r="H10" s="5102" t="s">
+      <c r="H10" s="5537" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="2648"/>
-      <c r="J10" s="5113" t="s">
-        <v>114</v>
+      <c r="J10" s="5548" t="s">
+        <v>209</v>
       </c>
-      <c r="K10" s="5124" t="s">
+      <c r="K10" s="5559" t="s">
         <v>115</v>
       </c>
-      <c r="L10" t="s" s="5135">
+      <c r="L10" t="s" s="5570">
         <v>198</v>
       </c>
       <c r="U10" s="8"/>
@@ -22655,32 +23993,32 @@
     <row r="11">
       <c r="A11" s="22"/>
       <c r="B11"/>
-      <c r="C11" s="5049" t="s">
+      <c r="C11" s="5484" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="5060" t="s">
+      <c r="D11" s="5495" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="5070" t="s">
+      <c r="E11" s="5505" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="5081" t="s">
-        <v>126</v>
+      <c r="F11" s="5516" t="s">
+        <v>116</v>
       </c>
-      <c r="G11" s="5092" t="s">
-        <v>127</v>
+      <c r="G11" s="5527" t="s">
+        <v>117</v>
       </c>
-      <c r="H11" s="5103" t="s">
+      <c r="H11" s="5538" t="s">
         <v>118</v>
       </c>
       <c r="I11" s="2649"/>
-      <c r="J11" s="5114" t="s">
-        <v>119</v>
+      <c r="J11" s="5549" t="s">
+        <v>210</v>
       </c>
-      <c r="K11" s="5125" t="s">
+      <c r="K11" s="5560" t="s">
         <v>120</v>
       </c>
-      <c r="L11" t="s" s="5136">
+      <c r="L11" t="s" s="5571">
         <v>199</v>
       </c>
       <c r="U11" s="8"/>
@@ -22694,32 +24032,32 @@
     <row r="12">
       <c r="A12" s="22"/>
       <c r="B12"/>
-      <c r="C12" s="5050" t="s">
+      <c r="C12" s="5485" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="5061" t="s">
+      <c r="D12" s="5496" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="5071" t="s">
+      <c r="E12" s="5506" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="5082" t="s">
-        <v>106</v>
+      <c r="F12" s="5517" t="s">
+        <v>121</v>
       </c>
-      <c r="G12" s="5093" t="s">
-        <v>107</v>
+      <c r="G12" s="5528" t="s">
+        <v>122</v>
       </c>
-      <c r="H12" s="5104" t="s">
+      <c r="H12" s="5539" t="s">
         <v>123</v>
       </c>
       <c r="I12" s="2650"/>
-      <c r="J12" s="5115" t="s">
-        <v>124</v>
+      <c r="J12" s="5550" t="s">
+        <v>211</v>
       </c>
-      <c r="K12" s="5126" t="s">
+      <c r="K12" s="5561" t="s">
         <v>125</v>
       </c>
-      <c r="L12" t="s" s="5137">
+      <c r="L12" t="s" s="5572">
         <v>200</v>
       </c>
       <c r="U12" s="8"/>
@@ -22733,32 +24071,32 @@
     <row r="13">
       <c r="A13" s="22"/>
       <c r="B13"/>
-      <c r="C13" s="5051" t="s">
+      <c r="C13" s="5486" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="5062" t="s">
+      <c r="D13" s="5497" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="5072" t="s">
+      <c r="E13" s="5507" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="5083" t="s">
-        <v>101</v>
+      <c r="F13" s="5518" t="s">
+        <v>126</v>
       </c>
-      <c r="G13" s="5094" t="s">
-        <v>102</v>
+      <c r="G13" s="5529" t="s">
+        <v>127</v>
       </c>
-      <c r="H13" s="5105" t="s">
+      <c r="H13" s="5540" t="s">
         <v>128</v>
       </c>
       <c r="I13" s="2651"/>
-      <c r="J13" s="5116" t="s">
-        <v>129</v>
+      <c r="J13" s="5551" t="s">
+        <v>212</v>
       </c>
-      <c r="K13" s="5127" t="s">
+      <c r="K13" s="5562" t="s">
         <v>130</v>
       </c>
-      <c r="L13" t="s" s="5138">
+      <c r="L13" t="s" s="5573">
         <v>201</v>
       </c>
       <c r="U13" s="8"/>

</xml_diff>